<commit_message>
fix the problem about RECORD and mircophone
</commit_message>
<xml_diff>
--- a/app_permission.xlsx
+++ b/app_permission.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ict\My_Project\Security\VR_Security_with_GPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1EA3CE-01F5-450B-B75D-DD9503FFE290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29B1EAE-046C-4831-A7C7-525209FDFBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="402">
   <si>
     <t>序号</t>
   </si>
@@ -427,85 +427,63 @@
     <t>多合一运动_All-in-OneSports_0.9.5</t>
   </si>
   <si>
-    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="29" ns0:compileSdkVersionCodename="10" ns0:installLocation="auto" package="com.Futuretown.Cloudlands2" platformBuildVersionCode="29" platformBuildVersionName="10"&gt;
+    <t>一场这是一个多人联机游戏。比赛10项运动！■ 丰富的运动项目体验-棒球、射箭、乒乓球、篮球、保龄球、羽毛球、高尔夫、飞镖、台球、拳击■ 多人实时PvP-拳击、棒球和乒乓球还不受支持■ 通过高级物理实现逼真的虚拟运动体验■ 播放器定制■ 简单的用户界面和简单的控制可以帮助任何人玩■ 从初学者到专业人士有5种不同的困难*比赛形式与奥运会官方规则相同，因此你可以学习运动训练和规则。*适用于由于体育设施和天气条件而必须在室内进行的虚拟现实体育教室。</t>
+  </si>
+  <si>
+    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="23" ns0:compileSdkVersionCodename="6.0-2438415" ns0:installLocation="auto" package="com.Appnori.AllInOneSports" platformBuildVersionCode="23" platformBuildVersionName="6.0-2438415"&gt;
+    &lt;supports-screens ns0:anyDensity="true" ns0:largeScreens="true" ns0:normalScreens="true" ns0:smallScreens="true" ns0:xlargeScreens="true" /&gt;
     &lt;uses-permission ns0:name="android.permission.INTERNET" /&gt;
-    &lt;uses-permission ns0:name="android.permission.ACCESS_WIFI_STATE" /&gt;
     &lt;uses-permission ns0:name="android.permission.ACCESS_NETWORK_STATE" /&gt;
     &lt;uses-permission ns0:name="android.permission.VIBRATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.SYSTEM_ALERT_WINDOW" /&gt;
+    &lt;uses-permission ns0:name="android.permission.READ_EXTERNAL_STORAGE" /&gt;
     &lt;uses-permission ns0:name="android.permission.WRITE_EXTERNAL_STORAGE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.READ_EXTERNAL_STORAGE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_MEDIA_STORAGE" /&gt;
     &lt;uses-permission ns0:name="android.permission.WRITE_SETTINGS" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_SECURE_SETTINGS" /&gt;
     &lt;uses-permission ns0:name="android.permission.CHANGE_CONFIGURATION" /&gt;
     &lt;uses-permission ns0:name="android.permission.BLUETOOTH" /&gt;
     &lt;uses-permission ns0:name="android.permission.BLUETOOTH_ADMIN" /&gt;
     &lt;uses-permission ns0:name="android.permission.INJECT_EVENTS" /&gt;
-    &lt;uses-permission ns0:name="android.permission.RECORD_AUDIO" /&gt;
-    &lt;supports-screens ns0:anyDensity="true" ns0:largeScreens="true" ns0:normalScreens="true" ns0:smallScreens="true" ns0:xlargeScreens="true" /&gt;
+    &lt;uses-permission ns0:name="android.permission.DEVICE_POWER" /&gt;
     &lt;uses-feature ns0:glEsVersion="0x00030000" /&gt;
     &lt;supports-gl-texture ns0:name="GL_KHR_texture_compression_astc_ldr" /&gt;
+    &lt;uses-permission ns0:name="android.permission.RECORD_AUDIO" /&gt;
+    &lt;uses-permission ns0:name="android.permission.MODIFY_AUDIO_SETTINGS" /&gt;
     &lt;uses-feature ns0:name="android.hardware.microphone" ns0:required="false" /&gt;
     &lt;uses-feature ns0:name="android.hardware.touchscreen" ns0:required="false" /&gt;
     &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch" ns0:required="false" /&gt;
     &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch.distinct" ns0:required="false" /&gt;
-    &lt;uses-permission ns0:name="android.permission.MODIFY_AUDIO_SETTINGS" /&gt;
     &lt;uses-permission ns0:name="android.permission.REORDER_TASKS" /&gt;
     &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_STATE" /&gt;
-    &lt;application ns0:allowBackup="true" ns0:icon="@mipmap/app_icon" ns0:label="@string/app_name" ns0:networkSecurityConfig="@xml/network_security_config" ns0:requestLegacyExternalStorage="true" ns0:roundIcon="@mipmap/app_icon_round" ns0:supportsRtl="true" ns0:theme="@android:style/Theme.Black.NoTitleBar.Fullscreen" ns0:usesCleartextTraffic="true"&gt;
-        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="Unity_2.8.10.4" /&gt;
-        &lt;meta-data ns0:name="pvr.app.type" ns0:value="vr" /&gt;
-        &lt;meta-data ns0:name="pvr.display.orientation" ns0:value="180" /&gt;
-        &lt;activity ns0:configChanges="density|fontScale|keyboard|keyboardHidden|layoutDirection|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:label="@string/app_name" ns0:launchMode="singleTask" ns0:name="com.unity3d.player.UnityPlayerNativeActivityPico" ns0:screenOrientation="landscape"&gt;
+    &lt;uses-permission ns0:name="android.permission.ACCESS_WIFI_STATE" /&gt;
+    &lt;application ns0:allowBackup="true" ns0:icon="@mipmap/app_icon" ns0:label="@string/app_name" ns0:supportsRtl="true"&gt;
+        &lt;activity ns0:configChanges="density|fontScale|keyboard|keyboardHidden|layoutDirection|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:launchMode="singleTask" ns0:name="com.unity3d.player.UnityPlayerActivity" ns0:screenOrientation="landscape" ns0:theme="@style/UnityThemeSelector"&gt;
             &lt;intent-filter&gt;
                 &lt;action ns0:name="android.intent.action.MAIN" /&gt;
                 &lt;category ns0:name="android.intent.category.LAUNCHER" /&gt;
             &lt;/intent-filter&gt;
             &lt;meta-data ns0:name="unityplayer.UnityActivity" ns0:value="true" /&gt;
-            &lt;meta-data ns0:name="unityplayer.ForwardNativeEventsToDalvik" ns0:value="false" /&gt;
+            &lt;meta-data ns0:name="android.notch_support" ns0:value="true" /&gt;
         &lt;/activity&gt;
-        &lt;activity ns0:configChanges="keyboard|keyboardHidden|orientation|screenSize" ns0:name="com.pico.loginpaysdk.UnityAuthInterface" ns0:screenOrientation="landscape" /&gt;
-        &lt;activity ns0:configChanges="keyboardHidden|orientation" ns0:exported="false" ns0:name="com.pico.loginpaysdk.component.PicoSDKBrowser" ns0:windowSoftInputMode="adjustResize" /&gt;
-        &lt;service ns0:name="com.picovr.hummingbirdsvc.AutoConnectService"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="com.picovr.hummingbirdsvc.AutoConnectService" /&gt;
-            &lt;/intent-filter&gt;
-        &lt;/service&gt;
-        &lt;service ns0:name="com.picovr.picovrlib.hummingbird.HummingBirdControllerService" ns0:process=":remote"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="com.picovr.picovrlib.humingbird.HumingBirdAIDLService" /&gt;
-            &lt;/intent-filter&gt;
-        &lt;/service&gt;
-        &lt;meta-data ns0:name="pico_merchant_id" ns0:value="2133" /&gt;
-        &lt;meta-data ns0:name="pico_app_id" ns0:value="53e5dcf91a261edd03f4e4cd95aeddf2" /&gt;
-        &lt;meta-data ns0:name="pico_app_key" ns0:value="f01a27920975b4917df3464bf3d3f0ef" /&gt;
-        &lt;meta-data ns0:name="pico_pay_key" ns0:value="ca4d982102d445e1d3ab0632b5184e9d" /&gt;
-        &lt;meta-data ns0:name="pico_redirectUrl" ns0:value="http://www.picovr.com" /&gt;
-        &lt;meta-data ns0:name="pico_merchant_id_foreign" ns0:value="2133" /&gt;
-        &lt;meta-data ns0:name="pico_app_id_foreign" ns0:value="53e5dcf91a261edd03f4e4cd95aeddf2" /&gt;
-        &lt;meta-data ns0:name="pico_app_key_foreign" ns0:value="f01a27920975b4917df3464bf3d3f0ef" /&gt;
-        &lt;meta-data ns0:name="pico_pay_key_foreign" ns0:value="ca4d982102d445e1d3ab0632b5184e9d" /&gt;
+        &lt;meta-data ns0:name="pico_app_id" ns0:value="50fdd4bd8916f7260f449032daad891a" /&gt;
+        &lt;meta-data ns0:name="pico_app_key" ns0:value="c848563d6d3890f62d377266c138b3ed" /&gt;
+        &lt;meta-data ns0:name="pico_scope" ns0:value="get_user_info" /&gt;
+        &lt;meta-data ns0:name="pico_merchant_id" ns0:value="2182" /&gt;
+        &lt;meta-data ns0:name="pico_pay_key" ns0:value="84280f6496aad4a5ad20e8a163a0137d" /&gt;
+        &lt;meta-data ns0:name="pico_app_id_foreign" ns0:value="c6a85a1abdf3639a799c344fb700dce3" /&gt;
+        &lt;meta-data ns0:name="pico_app_key_foreign" ns0:value="c6a85a1abdf3639a799c344fb700dce3" /&gt;
         &lt;meta-data ns0:name="pico_scope_foreign" ns0:value="get_user_info" /&gt;
-        &lt;meta-data ns0:name="pico_scope" ns0:value="get_user_info" /&gt;
-        &lt;meta-data ns0:name="com.pvr.instructionset" ns0:value="32" /&gt;
-        &lt;meta-data ns0:name="platform_logo" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="LoadingContent" ns0:resource="@string/loading" /&gt;
-        &lt;meta-data ns0:name="loadingcolor" ns0:resource="@color/custom" /&gt;
-        &lt;meta-data ns0:name="loadingtextsize" ns0:value="16" /&gt;
-        &lt;meta-data ns0:name="loadingwidth" ns0:value="500" /&gt;
-        &lt;meta-data ns0:name="loadingheight" ns0:value="100" /&gt;
-        &lt;meta-data ns0:name="loadingmarquee" ns0:value="1" /&gt;
-        &lt;meta-data ns0:name="bottommargin" ns0:value="100" /&gt;
-        &lt;meta-data ns0:name="marqueecount" ns0:value="10" /&gt;
-        &lt;meta-data ns0:name="loadingalign" ns0:value="left" /&gt;
-        &lt;meta-data ns0:name="com.pvr.hmd.trackingmode" ns0:value="6dof" /&gt;
-        &lt;meta-data ns0:name="isPUI" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="enable_eyetracking" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="enable_cpt" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="platform_high" ns0:value="1" /&gt;
-        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="1" /&gt;
-        &lt;meta-data ns0:name="MSAA" ns0:value="2" /&gt;
-        &lt;meta-data ns0:name="unity.build-id" ns0:value="573f1465-5bd5-49db-9e45-46b6e267f34b" /&gt;
+        &lt;meta-data ns0:name="pico_merchant_id_foreign" ns0:value="2182" /&gt;
+        &lt;meta-data ns0:name="pico_pay_key_foreign" ns0:value="c85da0b6c8da4c99c1aa4fc3c8cc2123" /&gt;
         &lt;meta-data ns0:name="unity.splash-mode" ns0:value="0" /&gt;
         &lt;meta-data ns0:name="unity.splash-enable" ns0:value="true" /&gt;
+        &lt;meta-data ns0:name="notch.config" ns0:value="portrait|landscape" /&gt;
+        &lt;meta-data ns0:name="unity.build-id" ns0:value="fc46f6a9-56c5-4745-9a11-98d504a882c7" /&gt;
+        &lt;meta-data ns0:name="pvr.app.type" ns0:value="vr" /&gt;
+        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="XR Platform_2.0.4.3" /&gt;
+        &lt;meta-data ns0:name="enable_cpt" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="1" /&gt;
         &lt;activity ns0:excludeFromRecents="true" ns0:exported="true" ns0:launchMode="singleTask" ns0:name="com.pico.loginpaysdk.auth.TransferStationActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar"&gt;
             &lt;intent-filter&gt;
                 &lt;action ns0:name="com.pico.loginpaysdk.intent.action.AuthCallback" /&gt;
@@ -525,97 +503,28 @@
     <t>启示骑士 是一个 VR 街机摩托车游戏，您必须在高速荒地公路上占优势，避免敌对交通，并继续生存，飞速行驶和骑行！特点 启示录骑士 - VR自行车赛车游戏 Android的：•20级纯VR肾上腺素•5辆摩托车可提供数十种升级•完整的虚拟现实环境•游戏手柄和运动控制器支持。</t>
   </si>
   <si>
-    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="30" ns0:compileSdkVersionCodename="11" ns0:installLocation="auto" package="com.vrm.aporiderNeo2" platformBuildVersionCode="69" platformBuildVersionName="1.7.8"&gt;
-    &lt;uses-feature ns0:glEsVersion="0x00030001" ns0:required="true" /&gt;
-    &lt;uses-permission ns0:name="android.permission.INTERNET" /&gt;
-    &lt;uses-permission ns0:name="android.permission.WRITE_EXTERNAL_STORAGE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.ACCESS_NETWORK_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.WAKE_LOCK" /&gt;
-    &lt;uses-permission ns0:name="com.android.vending.CHECK_LICENSE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.ACCESS_WIFI_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.MODIFY_AUDIO_SETTINGS" /&gt;
-    &lt;uses-permission ns0:name="android.permission.VIBRATE" /&gt;
-    &lt;supports-gl-texture ns0:name="GL_KHR_texture_compression_astc_ldr" /&gt;
-    &lt;uses-permission ns0:name="android.permission.READ_EXTERNAL_STORAGE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.WRITE_SETTINGS" /&gt;
-    &lt;uses-permission ns0:name="android.permission.CHANGE_CONFIGURATION" /&gt;
-    &lt;uses-permission ns0:name="android.permission.BLUETOOTH" /&gt;
-    &lt;uses-permission ns0:name="android.permission.BLUETOOTH_ADMIN" /&gt;
-    &lt;uses-permission ns0:name="android.permission.INJECT_EVENTS" /&gt;
-    &lt;application ns0:debuggable="true" ns0:hardwareAccelerated="false" ns0:hasCode="true" ns0:icon="@drawable/icon" ns0:label="@string/app_name" ns0:name="com.epicgames.ue4.GameApplication" ns0:requestLegacyExternalStorage="true"&gt;
-        &lt;activity ns0:configChanges="keyboard|keyboardHidden|navigation|orientation|screenSize" ns0:debuggable="true" ns0:hardwareAccelerated="false" ns0:label="@string/app_name" ns0:launchMode="singleTask" ns0:name="com.epicgames.ue4.SplashActivity" ns0:screenOrientation="landscape" ns0:theme="@style/UE4SplashTheme"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="android.intent.action.MAIN" /&gt;
-                &lt;category ns0:name="android.intent.category.LAUNCHER" /&gt;
-            &lt;/intent-filter&gt;
-        &lt;/activity&gt;
-        &lt;activity ns0:configChanges="keyboard|keyboardHidden|navigation|orientation|screenSize" ns0:debuggable="true" ns0:hardwareAccelerated="false" ns0:label="@string/app_name" ns0:launchMode="singleTask" ns0:name="com.epicgames.ue4.GameActivity" ns0:resizeableActivity="false" ns0:screenOrientation="landscape" ns0:theme="@style/UE4SplashTheme"&gt;
-            &lt;meta-data ns0:name="android.app.lib_name" ns0:value="UE4" /&gt;
-        &lt;/activity&gt;
-        &lt;activity ns0:configChanges="keyboard|keyboardHidden|navigation|orientation|screenSize" ns0:hardwareAccelerated="false" ns0:name="com.vrm.aporiderNeo2.DownloaderActivity" ns0:screenOrientation="landscape" ns0:theme="@style/UE4SplashTheme" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.EngineVersion" ns0:value="4.24.3" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.EngineBranch" ns0:value="++UE4+Release-4.24" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.ProjectVersion" ns0:value="2.5.1" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.DepthBufferPreference" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bPackageDataInsideApk" ns0:value="true" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bVerifyOBBOnStartUp" ns0:value="false" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bShouldHideUI" ns0:value="true" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.ProjectName" ns0:value="ApocalypseRider" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.AppType" ns0:value="" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bHasOBBFiles" ns0:value="true" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.BuildConfiguration" ns0:value="Development" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.CookedFlavors" ns0:value="ASTC" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bValidateTextureFormats" ns0:value="true" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bUseExternalFilesDir" ns0:value="false" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bPublicLogFiles" ns0:value="false" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bUseDisplayCutout" ns0:value="false" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bAllowIMU" ns0:value="true" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bSupportsVulkan" ns0:value="false" /&gt;
-        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.StartupPermissions" ns0:value="" /&gt;
-        &lt;meta-data ns0:name="com.google.android.gms.games.APP_ID" ns0:value="@string/app_id" /&gt;
-        &lt;meta-data ns0:name="com.google.android.gms.version" ns0:value="@integer/google_play_services_version" /&gt;
-        &lt;service ns0:name="com.vrm.aporiderNeo2.OBBDownloaderService" /&gt;
-        &lt;receiver ns0:name="com.vrm.aporiderNeo2.AlarmReceiver" /&gt;
-        &lt;receiver ns0:name="com.epicgames.ue4.LocalNotificationReceiver" /&gt;
-        &lt;receiver ns0:exported="true" ns0:name="com.epicgames.ue4.MulticastBroadcastReceiver"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="com.android.vending.INSTALL_REFERRER" /&gt;
-            &lt;/intent-filter&gt;
-        &lt;/receiver&gt;
-        &lt;meta-data ns0:name="android.max_aspect" ns0:value="2100000.0" /&gt;
-        &lt;activity ns0:configChanges="keyboard|keyboardHidden|navigation|orientation|screenSize" ns0:excludeFromRecents="true" ns0:exported="true" ns0:hardwareAccelerated="false" ns0:launchMode="singleTask" ns0:name="com.pico.loginpaysdk.auth.TransferStationActivity" ns0:screenOrientation="landscape" ns0:theme="@android:style/Theme.Translucent.NoTitleBar"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="com.pico.loginpaysdk.intent.action.AuthCallback" /&gt;
-                &lt;category ns0:name="android.intent.category.DEFAULT" /&gt;
-            &lt;/intent-filter&gt;
-        &lt;/activity&gt;
-        &lt;meta-data ns0:name="pico_app_id" ns0:value="6a3e998619ccfdb1ef114145f3ad7224" /&gt;
-        &lt;meta-data ns0:name="pico_app_key" ns0:value="" /&gt;
-        &lt;meta-data ns0:name="pico_scope" ns0:value="get_user_info" /&gt;
-        &lt;meta-data ns0:name="pico_merchant_id" ns0:value="" /&gt;
-        &lt;meta-data ns0:name="pico_pay_key" ns0:value="" /&gt;
-        &lt;meta-data ns0:name="pvr.app.type" ns0:value="vr" /&gt;
-        &lt;meta-data ns0:name="pvr.display.orientation" ns0:value="180" /&gt;
-        &lt;meta-data ns0:name="platform_logo" ns0:value="1" /&gt;
-        &lt;meta-data ns0:name="loadingtextsize" ns0:value="16" /&gt;
-        &lt;meta-data ns0:name="loadingwidth" ns0:value="500" /&gt;
-        &lt;meta-data ns0:name="loadingheight" ns0:value="100" /&gt;
-        &lt;meta-data ns0:name="loadingmarquee" ns0:value="1" /&gt;
-        &lt;meta-data ns0:name="bottommargin" ns0:value="100" /&gt;
-        &lt;meta-data ns0:name="marqueecount" ns0:value="10" /&gt;
-        &lt;meta-data ns0:name="loadingalign" ns0:value="left" /&gt;
-        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="UE4_1.2.5.5" /&gt;
-        &lt;meta-data ns0:name="com.pvr.hmd.trackingmode" ns0:value="6dof" /&gt;
-        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="1" /&gt;
-        &lt;activity ns0:excludeFromRecents="true" ns0:exported="false" ns0:name="com.google.android.gms.auth.api.signin.internal.SignInHubActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar" /&gt;
-        &lt;service ns0:exported="true" ns0:name="com.google.android.gms.auth.api.signin.RevocationBoundService" ns0:permission="com.google.android.gms.auth.api.signin.permission.REVOCATION_NOTIFICATION" /&gt;
-        &lt;provider ns0:authorities="com.vrm.aporiderNeo2.lifecycle-trojan" ns0:exported="false" ns0:multiprocess="true" ns0:name="android.arch.lifecycle.ProcessLifecycleOwnerInitializer" /&gt;
-        &lt;activity ns0:exported="false" ns0:name="com.google.android.gms.common.api.GoogleApiActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar" /&gt;
-    &lt;/application&gt;
-&lt;/manifest&gt;</t>
-  </si>
-  <si>
     <t>太空健身计划_SpaceFitness_1.0.1</t>
+  </si>
+  <si>
+    <t>【游戏名称】：Space Fitness【游戏类型】：运动【游戏平台】：pico【游戏模式】：原生VR游戏（定位控制器）【游戏语言】：多国语言游戏容量】：143MB【游戏介绍】：关于这款游戏在太空中，飞船突发意外，你需要几岁各式各样的陨石来通过不同挑战。《太空健身计划》集健身与游戏于一体，在这个广阔的太空中，你可以享受无限挑战乐趣。</t>
+  </si>
+  <si>
+    <t>Based on the permissions and features mentioned, the sensitive permissions and features that should not be requested are:
+Sensitive permissions:
+- android.permission.BLUETOOTH
+- android.permission.BLUETOOTH_ADMIN
+- android.permission.INJECT_EVENTS
+- android.permission.CHANGE_WIFI_MULTICAST_STATE
+- android.permission.ACCESS_FINE_LOCATION
+- android.permission.CAMERA
+- android.permission.RECORD_AUDIO
+Sensitive features:
+- android.hardware.location.gps
+- android.hardware.location
+- android.hardware.camera
+- android.hardware.camera.autofocus
+- android.hardware.camera.front
+- android.hardware.microphone</t>
   </si>
   <si>
     <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:installLocation="internalOnly" package="com.gvr.SpaceFitness"&gt;
@@ -731,211 +640,13 @@
     <t>这个游戏是一款模拟经营一家店的游戏，不过我不是店长。而是打杂的实习生啊！来了顾客要了解他想吃什么，然后自己做出来给顾客吃，手忙脚乱的感觉有木有，终于知道饭店实习生是有多么的辛苦了。还要定期打扫卫生，还有大细菌boss挑战，体验忙碌的一天。这个游戏让我想到了童年时光，记得那时候没有什么玩具，和小伙伴们用泥巴石头还有草树叶什么的当食物，一起玩过家家的游戏。哈哈，这是一款不错的游戏价格也便宜。</t>
   </si>
   <si>
-    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="29" ns0:compileSdkVersionCodename="10" ns0:installLocation="preferExternal" package="com.hunandamao.xiaochidian" platformBuildVersionCode="29" platformBuildVersionName="10"&gt;
-    &lt;supports-screens ns0:anyDensity="true" ns0:largeScreens="true" ns0:normalScreens="true" ns0:smallScreens="true" ns0:xlargeScreens="true" /&gt;
-    &lt;uses-permission ns0:name="android.permission.ACCESS_NETWORK_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.INTERNET" /&gt;
-    &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_MULTICAST_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.WRITE_EXTERNAL_STORAGE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.WRITE_SETTINGS" /&gt;
-    &lt;uses-permission ns0:name="android.permission.READ_EXTERNAL_STORAGE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.REORDER_TASKS" /&gt;
-    &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.ACCESS_WIFI_STATE" /&gt;
-    &lt;uses-feature ns0:glEsVersion="0x00030000" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.touchscreen" ns0:required="false" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch" ns0:required="false" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch.distinct" ns0:required="false" /&gt;
-    &lt;application ns0:allowBackup="true" ns0:icon="@mipmap/app_icon" ns0:label="@string/app_name" ns0:requestLegacyExternalStorage="true" ns0:supportsRtl="true" ns0:usesCleartextTraffic="true"&gt;
-        &lt;meta-data ns0:name="unity.builder" ns0:value="\ 12369761376126" /&gt;
-        &lt;activity ns0:configChanges="density|fontScale|keyboard|keyboardHidden|layoutDirection|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:launchMode="singleTask" ns0:name="com.unity3d.player.UnityPlayerActivity" ns0:screenOrientation="landscape" ns0:theme="@style/UnityThemeSelector"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="android.intent.action.MAIN" /&gt;
-                &lt;category ns0:name="android.intent.category.LAUNCHER" /&gt;
-            &lt;/intent-filter&gt;
-            &lt;meta-data ns0:name="unityplayer.UnityActivity" ns0:value="true" /&gt;
-            &lt;meta-data ns0:name="android.notch_support" ns0:value="true" /&gt;
-            &lt;meta-data ns0:name="android.notch_support" ns0:value="true" /&gt;
-        &lt;/activity&gt;
-        &lt;meta-data ns0:name="unity.splash-mode" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="unity.splash-enable" ns0:value="true" /&gt;
-        &lt;meta-data ns0:name="notch.config" ns0:value="portrait|landscape" /&gt;
-        &lt;meta-data ns0:name="unity.build-id" ns0:value="c3dbb196-3f63-41ea-8111-f0eb3e5af3e5" /&gt;
-        &lt;meta-data ns0:name="pvr.app.type" ns0:value="vr" /&gt;
-        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="XR Platform_1.2.4.7" /&gt;
-        &lt;meta-data ns0:name="enable_cpt" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="pico_merchant_id" ns0:value="5246" /&gt;
-        &lt;meta-data ns0:name="pico_app_id" ns0:value="c2a8870494a2005b73e87982f1f640aa" /&gt;
-        &lt;meta-data ns0:name="pico_app_key" ns0:value="16562ffe3bcedccd3da2395e50a8dc98" /&gt;
-        &lt;meta-data ns0:name="pico_pay_key" ns0:value="732f28f75f39fefd0a4262e640be0351" /&gt;
-        &lt;meta-data ns0:name="pico_app_id_foreign" ns0:value="81e6b29509fad6ee4cb9edb6b4e49d22" /&gt;
-        &lt;meta-data ns0:name="pico_app_key_foreign" ns0:value="03fa8d947440587acdb45e10939e5e31" /&gt;
-        &lt;meta-data ns0:name="pico_scope_foreign" ns0:value="get_user_info" /&gt;
-        &lt;meta-data ns0:name="pico_pay_key_foreign" ns0:value="bfbaeffa08e4bac4410482aa29d4e00b" /&gt;
-        &lt;meta-data ns0:name="pico_merchant_id_foreign" ns0:value="3653" /&gt;
-        &lt;meta-data ns0:name="pico_redirectUrl" ns0:value="http://www.picovr.com" /&gt;
-        &lt;meta-data ns0:name="pico_scope" ns0:value="get_user_info" /&gt;
-        &lt;meta-data ns0:name="com.pvr.instructionset" ns0:value="32" /&gt;
-        &lt;activity ns0:excludeFromRecents="true" ns0:exported="true" ns0:launchMode="singleTask" ns0:name="com.pico.loginpaysdk.auth.TransferStationActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="com.pico.loginpaysdk.intent.action.AuthCallback" /&gt;
-                &lt;category ns0:name="android.intent.category.DEFAULT" /&gt;
-            &lt;/intent-filter&gt;
-        &lt;/activity&gt;
-    &lt;/application&gt;
-&lt;/manifest&gt;</t>
-  </si>
-  <si>
     <t>异星入侵_EnterVR_2.0</t>
   </si>
   <si>
     <t>《EnterVR》是一款集弓弩射击、塔防于一体的VR游戏。佩戴HTC VIVE，现在就可以借助能量水晶侵入异星生物的世界了，马上拿起弓弩、投掷道具、发动技能，对抗从海陆空各处涌来的怪物吧。劲敌步步紧逼！全方位攻击花样来袭！能量水晶攻守之战一触即发！摸清那些异星生物所拥有的神秘力量，配合引爆道具，团结中立生物，守护属于你的新世界吧！(游戏内有很多值得探索的隐藏玩法：比如射击水中的游鱼可以给水晶回血；你附近的小石块可以捡起来砸向怪物，既能造成伤害还能引爆场景TNT道具；如果射到陆上小兵的头盔，弓箭是会被反弹而无法造成伤害的哦！运用好这些特殊的策略，相信每次游玩都会给您带来不一样的惊喜的！)</t>
   </si>
   <si>
-    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="29" ns0:compileSdkVersionCodename="10" ns0:installLocation="preferExternal" package="com.CharmingGame.EnterVR" platformBuildVersionCode="29" platformBuildVersionName="10"&gt;
-    &lt;supports-screens ns0:anyDensity="true" ns0:largeScreens="true" ns0:normalScreens="true" ns0:smallScreens="true" ns0:xlargeScreens="true" /&gt;
-    &lt;uses-feature ns0:glEsVersion="0x00020000" /&gt;
-    &lt;uses-permission ns0:name="android.permission.INTERNET" /&gt;
-    &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_MULTICAST_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.WRITE_EXTERNAL_STORAGE" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.sensor.accelerometer" ns0:required="false" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.touchscreen" ns0:required="false" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch" ns0:required="false" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch.distinct" ns0:required="false" /&gt;
-    &lt;uses-permission ns0:name="android.permission.WRITE_SETTINGS" /&gt;
-    &lt;uses-permission ns0:name="android.permission.READ_EXTERNAL_STORAGE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.REORDER_TASKS" /&gt;
-    &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.ACCESS_NETWORK_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.ACCESS_WIFI_STATE" /&gt;
-    &lt;application ns0:allowBackup="true" ns0:icon="@mipmap/app_icon" ns0:label="@string/app_name" ns0:requestLegacyExternalStorage="true" ns0:supportsRtl="true"&gt;
-        &lt;activity ns0:configChanges="density|fontScale|keyboard|keyboardHidden|layoutDirection|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:launchMode="singleTask" ns0:name="com.unity3d.player.UnityPlayerActivity" ns0:screenOrientation="landscape" ns0:theme="@style/UnityThemeSelector"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="android.intent.action.MAIN" /&gt;
-                &lt;category ns0:name="android.intent.category.LAUNCHER" /&gt;
-            &lt;/intent-filter&gt;
-            &lt;meta-data ns0:name="unityplayer.UnityActivity" ns0:value="true" /&gt;
-            &lt;meta-data ns0:name="android.notch_support" ns0:value="true" /&gt;
-        &lt;/activity&gt;
-        &lt;meta-data ns0:name="unity.splash-mode" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="unity.splash-enable" ns0:value="true" /&gt;
-        &lt;meta-data ns0:name="notch.config" ns0:value="portrait|landscape" /&gt;
-        &lt;meta-data ns0:name="unity.build-id" ns0:value="6a9274e7-cc42-4866-8ca4-70caf29c4af9" /&gt;
-        &lt;meta-data ns0:name="pvr.app.type" ns0:value="vr" /&gt;
-        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="XR Platform_1.2.3.5" /&gt;
-        &lt;meta-data ns0:name="enable_cpt" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="0" /&gt;
-        &lt;activity ns0:excludeFromRecents="true" ns0:exported="true" ns0:launchMode="singleTask" ns0:name="com.pico.loginpaysdk.auth.TransferStationActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="com.pico.loginpaysdk.intent.action.AuthCallback" /&gt;
-                &lt;category ns0:name="android.intent.category.DEFAULT" /&gt;
-            &lt;/intent-filter&gt;
-        &lt;/activity&gt;
-        &lt;activity ns0:configChanges="fontScale|keyboard|keyboardHidden|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="true" ns0:name="com.unity3d.services.ads.adunit.AdUnitActivity" ns0:theme="@android:style/Theme.NoTitleBar.Fullscreen" /&gt;
-        &lt;activity ns0:configChanges="fontScale|keyboard|keyboardHidden|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="true" ns0:name="com.unity3d.services.ads.adunit.AdUnitTransparentActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar.Fullscreen" /&gt;
-        &lt;activity ns0:configChanges="fontScale|keyboard|keyboardHidden|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:name="com.unity3d.services.ads.adunit.AdUnitTransparentSoftwareActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar.Fullscreen" /&gt;
-        &lt;activity ns0:configChanges="fontScale|keyboard|keyboardHidden|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:name="com.unity3d.services.ads.adunit.AdUnitSoftwareActivity" ns0:theme="@android:style/Theme.NoTitleBar.Fullscreen" /&gt;
-    &lt;/application&gt;
-&lt;/manifest&gt;</t>
-  </si>
-  <si>
     <t>9月的晚餐_SepsDiner_8592_19</t>
-  </si>
-  <si>
-    <t>欢迎来到 Sep’s Diner，这是一家由您担任主厨的新汉堡餐厅！它真的会成为镇上最好的汉堡吗？现在就看你了！一层又一层，您的体验将增加，美食客户的数量也会增加。他们很匆忙，所以在他们离开之前尽快满足他们！
-饥饿和不耐烦，他们不会让您犯错误…… 细心和精确，以获得最大的利润！包括全新的甜点餐厅Sep’s Donut！游戏特色：· 2间餐厅· 包括 3 种游戏模式：定时、轻松、多人· 每家餐厅包括 27 个级别（定时/休闲 12 个，多人游戏 3 个）· 最多 4 名玩家的多人合作游戏· 紧张刺激的关卡！· 身临其境的音频氛围· 不耐烦的客户用有趣的声音· 美丽的风景和彩灯· 逐级增加难度· 超过 30 种不同的汉堡食谱组合！· 煎饼、甜甜圈、华夫饼、纸杯蛋糕、冰淇淋和奶昔！</t>
-  </si>
-  <si>
-    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="29" ns0:compileSdkVersionCodename="10" ns0:installLocation="auto" package="com.scale1.sepsdinerSolo" platformBuildVersionCode="29" platformBuildVersionName="10"&gt;
-    &lt;supports-screens ns0:anyDensity="true" ns0:largeScreens="true" ns0:normalScreens="true" ns0:smallScreens="true" ns0:xlargeScreens="true" /&gt;
-    &lt;uses-permission ns0:name="android.permission.WRITE_EXTERNAL_STORAGE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.READ_EXTERNAL_STORAGE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.BLUETOOTH" /&gt;
-    &lt;uses-permission ns0:name="android.permission.BLUETOOTH_ADMIN" /&gt;
-    &lt;uses-permission ns0:name="android.permission.INJECT_EVENTS" /&gt;
-    &lt;uses-permission ns0:name="android.permission.INTERNET" /&gt;
-    &lt;uses-permission ns0:name="android.permission.ACCESS_NETWORK_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.VIBRATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.WRITE_SETTINGS" /&gt;
-    &lt;uses-permission ns0:name="android.permission.CHANGE_CONFIGURATION" /&gt;
-    &lt;uses-feature ns0:glEsVersion="0x00030000" /&gt;
-    &lt;uses-permission ns0:name="android.permission.RECORD_AUDIO" /&gt;
-    &lt;uses-permission ns0:name="android.permission.MODIFY_AUDIO_SETTINGS" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.microphone" ns0:required="false" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.sensor.accelerometer" ns0:required="false" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.touchscreen" ns0:required="false" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch" ns0:required="false" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch.distinct" ns0:required="false" /&gt;
-    &lt;uses-permission ns0:name="android.permission.REORDER_TASKS" /&gt;
-    &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.ACCESS_WIFI_STATE" /&gt;
-    &lt;application ns0:allowBackup="true" ns0:debuggable="false" ns0:icon="@mipmap/app_icon" ns0:label="@string/app_name" ns0:requestLegacyExternalStorage="true" ns0:roundIcon="@mipmap/app_icon_round" ns0:supportsRtl="true" ns0:theme="@android:style/Theme.Black.NoTitleBar.Fullscreen"&gt;
-        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="Unity_2.8.9.12" /&gt;
-        &lt;meta-data ns0:name="pvr.app.type" ns0:value="vr" /&gt;
-        &lt;meta-data ns0:name="pvr.display.orientation" ns0:value="180" /&gt;
-        &lt;activity ns0:configChanges="density|fontScale|keyboard|keyboardHidden|layoutDirection|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:label="@string/app_name" ns0:launchMode="singleTask" ns0:name="com.unity3d.player.UnityPlayerNativeActivityPico" ns0:screenOrientation="landscape"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="android.intent.action.MAIN" /&gt;
-                &lt;category ns0:name="android.intent.category.LAUNCHER" /&gt;
-            &lt;/intent-filter&gt;
-            &lt;meta-data ns0:name="unityplayer.UnityActivity" ns0:value="true" /&gt;
-            &lt;meta-data ns0:name="unityplayer.ForwardNativeEventsToDalvik" ns0:value="false" /&gt;
-            &lt;meta-data ns0:name="android.notch_support" ns0:value="true" /&gt;
-        &lt;/activity&gt;
-        &lt;activity ns0:configChanges="keyboard|keyboardHidden|orientation|screenSize" ns0:name="com.pico.loginpaysdk.UnityAuthInterface" ns0:screenOrientation="landscape" /&gt;
-        &lt;activity ns0:configChanges="keyboardHidden|orientation" ns0:exported="false" ns0:name="com.pico.loginpaysdk.component.PicoSDKBrowser" ns0:windowSoftInputMode="adjustResize" /&gt;
-        &lt;service ns0:name="com.picovr.hummingbirdsvc.AutoConnectService"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="com.picovr.hummingbirdsvc.AutoConnectService" /&gt;
-            &lt;/intent-filter&gt;
-        &lt;/service&gt;
-        &lt;service ns0:name="com.picovr.picovrlib.hummingbird.HummingBirdControllerService" ns0:process=":remote"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="com.picovr.picovrlib.humingbird.HumingBirdAIDLService" /&gt;
-            &lt;/intent-filter&gt;
-        &lt;/service&gt;
-        &lt;meta-data ns0:name="com.pvr.instructionset" ns0:value="32" /&gt;
-        &lt;meta-data ns0:name="unityplayer.SkipPermissionsDialog" ns0:value="false" /&gt;
-        &lt;meta-data ns0:name="platform_logo" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="LoadingContent" ns0:resource="@string/loading" /&gt;
-        &lt;meta-data ns0:name="loadingcolor" ns0:resource="@color/custom" /&gt;
-        &lt;meta-data ns0:name="loadingtextsize" ns0:value="16" /&gt;
-        &lt;meta-data ns0:name="loadingwidth" ns0:value="500" /&gt;
-        &lt;meta-data ns0:name="loadingheight" ns0:value="100" /&gt;
-        &lt;meta-data ns0:name="loadingmarquee" ns0:value="1" /&gt;
-        &lt;meta-data ns0:name="bottommargin" ns0:value="100" /&gt;
-        &lt;meta-data ns0:name="marqueecount" ns0:value="10" /&gt;
-        &lt;meta-data ns0:name="loadingalign" ns0:value="left" /&gt;
-        &lt;meta-data ns0:name="com.pvr.hmd.trackingmode" ns0:value="6dof" /&gt;
-        &lt;meta-data ns0:name="isPUI" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="enable_eyetracking" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="enable_cpt" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="platform_high" ns0:value="1" /&gt;
-        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="1" /&gt;
-        &lt;meta-data ns0:name="pico_redirectUrl" ns0:value="http://www.picovr.com" /&gt;
-        &lt;meta-data ns0:name="pico_app_id" ns0:value="11638f51026498097f5a8938c9ee782a" /&gt;
-        &lt;meta-data ns0:name="pico_app_key" ns0:value="a9a79a522fa6fdb20a3a284ac3250769" /&gt;
-        &lt;meta-data ns0:name="pico_scope" ns0:value="get_user_info" /&gt;
-        &lt;meta-data ns0:name="pico_merchant_id" ns0:value="7230" /&gt;
-        &lt;meta-data ns0:name="pico_pay_key" ns0:value="af7153a5cdba32f20040b9b257f173a5" /&gt;
-        &lt;meta-data ns0:name="pico_app_id_foreign" ns0:value="11638f51026498097f5a8938c9ee782a" /&gt;
-        &lt;meta-data ns0:name="pico_app_key_foreign" ns0:value="a9a79a522fa6fdb20a3a284ac3250769" /&gt;
-        &lt;meta-data ns0:name="pico_scope_foreign" ns0:value="get_user_info" /&gt;
-        &lt;meta-data ns0:name="pico_merchant_id_foreign" ns0:value="7230" /&gt;
-        &lt;meta-data ns0:name="pico_pay_key_foreign" ns0:value="APP SECRET" /&gt;
-        &lt;meta-data ns0:name="unity.splash-mode" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="unity.splash-enable" ns0:value="true" /&gt;
-        &lt;meta-data ns0:name="notch.config" ns0:value="portrait|landscape" /&gt;
-        &lt;meta-data ns0:name="unity.build-id" ns0:value="ee1ef296-528d-4e67-834d-a02c999e78a8" /&gt;
-        &lt;activity ns0:excludeFromRecents="true" ns0:exported="true" ns0:launchMode="singleTask" ns0:name="com.pico.loginpaysdk.auth.TransferStationActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="com.pico.loginpaysdk.intent.action.AuthCallback" /&gt;
-                &lt;category ns0:name="android.intent.category.DEFAULT" /&gt;
-            &lt;/intent-filter&gt;
-        &lt;/activity&gt;
-    &lt;/application&gt;
-&lt;/manifest&gt;</t>
   </si>
   <si>
     <t>BeatBlaster_1.5</t>
@@ -950,93 +661,6 @@
 - 太空音乐竞技场 |使用耳机，享受美妙的节拍和音乐！
 - 挑战 |游戏中有首领，您有足够的勇气与他们战斗吗？
 - 更新 |我们将每月更新我们的游戏，为您带来新的内容。</t>
-  </si>
-  <si>
-    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="29" ns0:compileSdkVersionCodename="10" ns0:installLocation="auto" package="com.IvanovichGames.BeatBlaster" platformBuildVersionCode="29" platformBuildVersionName="10"&gt;
-    &lt;supports-screens ns0:anyDensity="true" ns0:largeScreens="true" ns0:normalScreens="true" ns0:smallScreens="true" ns0:xlargeScreens="true" /&gt;
-    &lt;uses-permission ns0:name="android.permission.INTERNET" /&gt;
-    &lt;uses-permission ns0:name="android.permission.ACCESS_NETWORK_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.VIBRATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.WRITE_EXTERNAL_STORAGE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.READ_EXTERNAL_STORAGE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.WRITE_SETTINGS" /&gt;
-    &lt;uses-permission ns0:name="android.permission.CHANGE_CONFIGURATION" /&gt;
-    &lt;uses-permission ns0:name="android.permission.BLUETOOTH" /&gt;
-    &lt;uses-permission ns0:name="android.permission.BLUETOOTH_ADMIN" /&gt;
-    &lt;uses-permission ns0:name="android.permission.INJECT_EVENTS" /&gt;
-    &lt;uses-feature ns0:glEsVersion="0x00030000" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.vulkan.version" ns0:required="false" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.touchscreen" ns0:required="false" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch" ns0:required="false" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch.distinct" ns0:required="false" /&gt;
-    &lt;uses-permission ns0:name="android.permission.REORDER_TASKS" /&gt;
-    &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.ACCESS_WIFI_STATE" /&gt;
-    &lt;uses-permission ns0:name="com.android.vending.CHECK_LICENSE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.WAKE_LOCK" /&gt;
-    &lt;application ns0:allowBackup="true" ns0:debuggable="false" ns0:extractNativeLibs="true" ns0:icon="@mipmap/app_icon" ns0:label="@string/app_name" ns0:requestLegacyExternalStorage="true" ns0:roundIcon="@mipmap/app_icon_round" ns0:supportsRtl="true" ns0:theme="@android:style/Theme.Black.NoTitleBar.Fullscreen"&gt;
-        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="Unity_2.8.9.12" /&gt;
-        &lt;meta-data ns0:name="pvr.app.type" ns0:value="vr" /&gt;
-        &lt;meta-data ns0:name="pvr.display.orientation" ns0:value="180" /&gt;
-        &lt;activity ns0:configChanges="density|fontScale|keyboard|keyboardHidden|layoutDirection|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:label="@string/app_name" ns0:launchMode="singleTask" ns0:name="com.unity3d.player.UnityPlayerNativeActivityPico" ns0:resizeableActivity="false" ns0:screenOrientation="landscape"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="android.intent.action.MAIN" /&gt;
-                &lt;category ns0:name="android.intent.category.LAUNCHER" /&gt;
-            &lt;/intent-filter&gt;
-            &lt;meta-data ns0:name="unityplayer.UnityActivity" ns0:value="true" /&gt;
-            &lt;meta-data ns0:name="unityplayer.ForwardNativeEventsToDalvik" ns0:value="false" /&gt;
-        &lt;/activity&gt;
-        &lt;activity ns0:configChanges="keyboard|keyboardHidden|orientation|screenSize" ns0:name="com.pico.loginpaysdk.UnityAuthInterface" ns0:screenOrientation="landscape" /&gt;
-        &lt;activity ns0:configChanges="keyboardHidden|orientation" ns0:exported="false" ns0:name="com.pico.loginpaysdk.component.PicoSDKBrowser" ns0:windowSoftInputMode="adjustResize" /&gt;
-        &lt;service ns0:name="com.picovr.hummingbirdsvc.AutoConnectService"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="com.picovr.hummingbirdsvc.AutoConnectService" /&gt;
-            &lt;/intent-filter&gt;
-        &lt;/service&gt;
-        &lt;service ns0:name="com.picovr.picovrlib.hummingbird.HummingBirdControllerService" ns0:process=":remote"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="com.picovr.picovrlib.humingbird.HumingBirdAIDLService" /&gt;
-            &lt;/intent-filter&gt;
-        &lt;/service&gt;
-        &lt;meta-data ns0:name="pico_merchant_id" ns0:value="81" /&gt;
-        &lt;meta-data ns0:name="pico_app_id" ns0:value="56898ecfc4a8f01dc518016fb7b1c0bc" /&gt;
-        &lt;meta-data ns0:name="pico_app_key" ns0:value="dc349716a16d8ef8061f8b62750c85ad" /&gt;
-        &lt;meta-data ns0:name="pico_pay_key" ns0:value="7f0c28552ea4427c03b67fdd66cf7e55" /&gt;
-        &lt;meta-data ns0:name="pico_redirectUrl" ns0:value="http://www.picovr.com" /&gt;
-        &lt;meta-data ns0:name="pico_scope" ns0:value="get_user_info" /&gt;
-        &lt;meta-data ns0:name="com.pvr.instructionset" ns0:value="32" /&gt;
-        &lt;meta-data ns0:name="platform_logo" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="LoadingContent" ns0:resource="@string/loading" /&gt;
-        &lt;meta-data ns0:name="loadingcolor" ns0:resource="@color/custom" /&gt;
-        &lt;meta-data ns0:name="loadingtextsize" ns0:value="16" /&gt;
-        &lt;meta-data ns0:name="loadingwidth" ns0:value="500" /&gt;
-        &lt;meta-data ns0:name="loadingheight" ns0:value="100" /&gt;
-        &lt;meta-data ns0:name="loadingmarquee" ns0:value="1" /&gt;
-        &lt;meta-data ns0:name="bottommargin" ns0:value="100" /&gt;
-        &lt;meta-data ns0:name="marqueecount" ns0:value="10" /&gt;
-        &lt;meta-data ns0:name="loadingalign" ns0:value="left" /&gt;
-        &lt;meta-data ns0:name="com.pvr.hmd.trackingmode" ns0:value="6dof" /&gt;
-        &lt;meta-data ns0:name="isPUI" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="enable_eyetracking" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="enable_cpt" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="platform_high" ns0:value="1" /&gt;
-        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="1" /&gt;
-        &lt;meta-data ns0:name="MSAA" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="unity.splash-mode" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="unity.splash-enable" ns0:value="true" /&gt;
-        &lt;meta-data ns0:name="unity.allow-resizable-window" ns0:value="false" /&gt;
-        &lt;meta-data ns0:name="unity.build-id" ns0:value="b8492c8a-f3aa-4abf-a368-2c6ccb496c52" /&gt;
-        &lt;activity ns0:excludeFromRecents="true" ns0:exported="true" ns0:launchMode="singleTask" ns0:name="com.pico.loginpaysdk.auth.TransferStationActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar"&gt;
-            &lt;intent-filter&gt;
-                &lt;action ns0:name="com.pico.loginpaysdk.intent.action.AuthCallback" /&gt;
-                &lt;category ns0:name="android.intent.category.DEFAULT" /&gt;
-            &lt;/intent-filter&gt;
-        &lt;/activity&gt;
-        &lt;activity ns0:name="com.unity3d.plugin.downloader.UnityDownloaderActivity" /&gt;
-        &lt;service ns0:name="com.unity3d.plugin.downloader.UnityDownloaderService" /&gt;
-        &lt;receiver ns0:name="com.unity3d.plugin.downloader.UnityAlarmReceiver" /&gt;
-    &lt;/application&gt;
-&lt;/manifest&gt;</t>
   </si>
   <si>
     <t>Cloudlands2高尔夫_1.31</t>
@@ -1143,58 +767,90 @@
     <t>《Faraland》是一款回合 制策略和角色扮演游戏。在游戏中，你可以使用你的英雄，通过学习强大的技能、收集稀有装备、招募军队、在地图上运动、捕获资源和加入战斗来与其他玩家竞争。游戏的灵感来自魔兽世界、最终幻想故事情节、地平线零黎明背景、口袋妖怪和最终幻想战术战斗系统以及EVE在线游戏-玩家可以互相做任何事情。</t>
   </si>
   <si>
-    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="23" ns0:compileSdkVersionCodename="6.0-2438415" ns0:installLocation="auto" package="com.odders.ohshape.pico.neo2" platformBuildVersionCode="30" platformBuildVersionName="11"&gt;
+    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="29" ns0:compileSdkVersionCodename="10" ns0:installLocation="auto" package="com.fxg.fernland" platformBuildVersionCode="29" platformBuildVersionName="10"&gt;
     &lt;supports-screens ns0:anyDensity="true" ns0:largeScreens="true" ns0:normalScreens="true" ns0:smallScreens="true" ns0:xlargeScreens="true" /&gt;
-    &lt;uses-feature ns0:glEsVersion="0x00030000" /&gt;
+    &lt;uses-permission ns0:name="android.permission.ACCESS_NETWORK_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.INTERNET" /&gt;
+    &lt;uses-permission ns0:name="android.permission.VIBRATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_EXTERNAL_STORAGE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.READ_EXTERNAL_STORAGE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_SETTINGS" /&gt;
+    &lt;uses-permission ns0:name="android.permission.CHANGE_CONFIGURATION" /&gt;
+    &lt;uses-permission ns0:name="android.permission.BLUETOOTH" /&gt;
+    &lt;uses-permission ns0:name="android.permission.BLUETOOTH_ADMIN" /&gt;
+    &lt;uses-permission ns0:name="android.permission.INJECT_EVENTS" /&gt;
+    &lt;uses-feature ns0:glEsVersion="0x00020000" /&gt;
+    &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_MULTICAST_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.RECORD_AUDIO" /&gt;
+    &lt;uses-permission ns0:name="android.permission.MODIFY_AUDIO_SETTINGS" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.microphone" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.sensor.accelerometer" ns0:required="false" /&gt;
     &lt;uses-feature ns0:name="android.hardware.touchscreen" ns0:required="false" /&gt;
     &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch" ns0:required="false" /&gt;
     &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch.distinct" ns0:required="false" /&gt;
-    &lt;uses-permission ns0:name="android.permission.WRITE_SETTINGS" /&gt;
     &lt;uses-permission ns0:name="android.permission.REORDER_TASKS" /&gt;
     &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.INTERNET" /&gt;
-    &lt;uses-permission ns0:name="android.permission.ACCESS_NETWORK_STATE" /&gt;
     &lt;uses-permission ns0:name="android.permission.ACCESS_WIFI_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.RECORD_AUDIO" /&gt;
-    &lt;uses-permission ns0:name="android.permission.MODIFY_AUDIO_SETTINGS" /&gt;
-    &lt;uses-permission ns0:name="android.permission.BLUETOOTH" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.microphone" ns0:required="false" /&gt;
-    &lt;uses-permission ns0:name="android.permission.WRITE_EXTERNAL_STORAGE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.READ_EXTERNAL_STORAGE" /&gt;
-    &lt;application ns0:allowBackup="true" ns0:icon="@mipmap/app_icon" ns0:label="@string/app_name" ns0:requestLegacyExternalStorage="true" ns0:supportsRtl="true" ns0:usesCleartextTraffic="true"&gt;
-        &lt;activity ns0:configChanges="density|fontScale|keyboard|keyboardHidden|layoutDirection|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:launchMode="singleTask" ns0:name="com.unity3d.player.UnityPlayerActivity" ns0:screenOrientation="landscape" ns0:theme="@style/UnityThemeSelector"&gt;
+    &lt;application ns0:allowBackup="true" ns0:debuggable="false" ns0:icon="@mipmap/app_icon" ns0:label="@string/app_name" ns0:requestLegacyExternalStorage="true" ns0:supportsRtl="true" ns0:theme="@android:style/Theme.Black.NoTitleBar.Fullscreen" ns0:usesCleartextTraffic="true"&gt;
+        &lt;meta-data ns0:name="unity.builder" ns0:value="\ 15668321425885" /&gt;
+        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="Unity_2.8.10.4" /&gt;
+        &lt;meta-data ns0:name="pvr.app.type" ns0:value="vr" /&gt;
+        &lt;meta-data ns0:name="pvr.display.orientation" ns0:value="180" /&gt;
+        &lt;activity ns0:configChanges="density|fontScale|keyboard|keyboardHidden|layoutDirection|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:label="@string/app_name" ns0:launchMode="singleTask" ns0:name="com.unity3d.player.UnityPlayerNativeActivityPico" ns0:screenOrientation="landscape"&gt;
             &lt;intent-filter&gt;
                 &lt;action ns0:name="android.intent.action.MAIN" /&gt;
                 &lt;category ns0:name="android.intent.category.LAUNCHER" /&gt;
             &lt;/intent-filter&gt;
             &lt;meta-data ns0:name="unityplayer.UnityActivity" ns0:value="true" /&gt;
-            &lt;meta-data ns0:name="android.notch_support" ns0:value="true" /&gt;
+            &lt;meta-data ns0:name="unityplayer.ForwardNativeEventsToDalvik" ns0:value="false" /&gt;
             &lt;meta-data ns0:name="android.notch_support" ns0:value="true" /&gt;
         &lt;/activity&gt;
+        &lt;activity ns0:configChanges="keyboard|keyboardHidden|orientation|screenSize" ns0:name="com.pico.loginpaysdk.UnityAuthInterface" ns0:screenOrientation="landscape" /&gt;
+        &lt;activity ns0:configChanges="keyboardHidden|orientation" ns0:exported="false" ns0:name="com.pico.loginpaysdk.component.PicoSDKBrowser" ns0:windowSoftInputMode="adjustResize" /&gt;
+        &lt;service ns0:name="com.picovr.hummingbirdsvc.AutoConnectService"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="com.picovr.hummingbirdsvc.AutoConnectService" /&gt;
+            &lt;/intent-filter&gt;
+        &lt;/service&gt;
+        &lt;service ns0:name="com.picovr.picovrlib.hummingbird.HummingBirdControllerService" ns0:process=":remote"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="com.picovr.picovrlib.humingbird.HumingBirdAIDLService" /&gt;
+            &lt;/intent-filter&gt;
+        &lt;/service&gt;
+        &lt;meta-data ns0:name="pico_merchant_id" ns0:value="81" /&gt;
+        &lt;meta-data ns0:name="pico_app_id" ns0:value="5a189befeb3b33f7df101fbecffe4f98" /&gt;
+        &lt;meta-data ns0:name="pico_app_key" ns0:value="25ba00fb73343ff1ec32e1c152fff291" /&gt;
+        &lt;meta-data ns0:name="pico_pay_key" ns0:value="d828c5d3a1cc11e6b7fe008cfaf3d930" /&gt;
+        &lt;meta-data ns0:name="pico_redirectUrl" ns0:value="http://www.picovr.com" /&gt;
+        &lt;meta-data ns0:name="pico_scope" ns0:value="get_user_info" /&gt;
+        &lt;meta-data ns0:name="com.pvr.instructionset" ns0:value="32" /&gt;
+        &lt;meta-data ns0:name="platform_logo" ns0:value="1" /&gt;
+        &lt;meta-data ns0:name="LoadingContent" ns0:resource="@string/loading" /&gt;
+        &lt;meta-data ns0:name="loadingcolor" ns0:resource="@color/custom" /&gt;
+        &lt;meta-data ns0:name="loadingtextsize" ns0:value="16" /&gt;
+        &lt;meta-data ns0:name="loadingwidth" ns0:value="500" /&gt;
+        &lt;meta-data ns0:name="loadingheight" ns0:value="100" /&gt;
+        &lt;meta-data ns0:name="loadingmarquee" ns0:value="1" /&gt;
+        &lt;meta-data ns0:name="bottommargin" ns0:value="100" /&gt;
+        &lt;meta-data ns0:name="marqueecount" ns0:value="10" /&gt;
+        &lt;meta-data ns0:name="loadingalign" ns0:value="left" /&gt;
+        &lt;meta-data ns0:name="com.pvr.hmd.trackingmode" ns0:value="6dof" /&gt;
+        &lt;meta-data ns0:name="isPUI" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="enable_eyetracking" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="enable_cpt" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="platform_high" ns0:value="1" /&gt;
+        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="MSAA" ns0:value="4" /&gt;
         &lt;meta-data ns0:name="unity.splash-mode" ns0:value="0" /&gt;
         &lt;meta-data ns0:name="unity.splash-enable" ns0:value="true" /&gt;
         &lt;meta-data ns0:name="notch.config" ns0:value="portrait|landscape" /&gt;
-        &lt;meta-data ns0:name="unity.build-id" ns0:value="0ea0d07a-9d72-4946-8645-e39c1750c105" /&gt;
-        &lt;meta-data ns0:name="pvr.app.type" ns0:value="vr" /&gt;
-        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="XR Platform_2.0.4.3" /&gt;
-        &lt;meta-data ns0:name="enable_cpt" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="1" /&gt;
-        &lt;meta-data ns0:name="pico_app_id" ns0:value="83a7cd05349ad5c38f5c8fa53466239b" /&gt;
-        &lt;meta-data ns0:name="pico_app_key" ns0:value="317b35cecd1fc75c3cb3e022deacd002" /&gt;
-        &lt;meta-data ns0:name="pico_scope" ns0:value="get_user_info" /&gt;
-        &lt;meta-data ns0:name="pico_pay_key" ns0:value="ae7b982818ff89a2f7b0fed2ffb4c048" /&gt;
-        &lt;meta-data ns0:name="pico_app_id_foreign" ns0:value="83a7cd05349ad5c38f5c8fa53466239b" /&gt;
-        &lt;meta-data ns0:name="pico_app_key_foreign" ns0:value="317b35cecd1fc75c3cb3e022deacd002" /&gt;
-        &lt;meta-data ns0:name="pico_scope_foreign" ns0:value="get_user_info" /&gt;
-        &lt;meta-data ns0:name="pico_pay_key_foreign" ns0:value="ae7b982818ff89a2f7b0fed2ffb4c048" /&gt;
+        &lt;meta-data ns0:name="unity.build-id" ns0:value="57e87611-a4d7-444e-aeb6-1da227bed2f2" /&gt;
         &lt;activity ns0:excludeFromRecents="true" ns0:exported="true" ns0:launchMode="singleTask" ns0:name="com.pico.loginpaysdk.auth.TransferStationActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar"&gt;
             &lt;intent-filter&gt;
                 &lt;action ns0:name="com.pico.loginpaysdk.intent.action.AuthCallback" /&gt;
                 &lt;category ns0:name="android.intent.category.DEFAULT" /&gt;
             &lt;/intent-filter&gt;
         &lt;/activity&gt;
-        &lt;activity ns0:name="com.yasirkula.unity.NativeShareCustomShareDialogActivity" ns0:theme="@style/Theme.NativeShareTransparent" /&gt;
-        &lt;provider ns0:authorities="com.odders.ohshape.pico.neo2.NativeShareContentProvider" ns0:exported="false" ns0:grantUriPermissions="true" ns0:name="com.yasirkula.unity.NativeShareContentProvider" /&gt;
         &lt;activity ns0:configChanges="fontScale|keyboard|keyboardHidden|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="true" ns0:name="com.unity3d.services.ads.adunit.AdUnitActivity" ns0:theme="@android:style/Theme.NoTitleBar.Fullscreen" /&gt;
         &lt;activity ns0:configChanges="fontScale|keyboard|keyboardHidden|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="true" ns0:name="com.unity3d.services.ads.adunit.AdUnitTransparentActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar.Fullscreen" /&gt;
         &lt;activity ns0:configChanges="fontScale|keyboard|keyboardHidden|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:name="com.unity3d.services.ads.adunit.AdUnitTransparentSoftwareActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar.Fullscreen" /&gt;
@@ -1375,11 +1031,150 @@
 • 跨平台在线排行榜</t>
   </si>
   <si>
+    <t>Based on the description and the mentioned permissions and features, the sensitive permissions that should not be requested are:
+- android.permission.REORDER_TASKS: This permission is not necessary for the functionality of the game.
+- android.permission.RECORD_AUDIO: This permission is not mentioned in the game description and may not be required for the gameplay.
+- android.permission.MODIFY_AUDIO_SETTINGS: This permission is not necessary for the gameplay.
+- android.permission.WRITE_EXTERNAL_STORAGE: This permission is not mentioned in the game description and may not be required for the gameplay.
+- android.permission.READ_EXTERNAL_STORAGE: This permission is not mentioned in the game description and may not be required for the gameplay.
+All other permissions mentioned in the question are related to the necessary functionality of the game, such as accessing network state, changing Wi-Fi state, and accessing touch screen and Bluetooth capabilities.</t>
+  </si>
+  <si>
+    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="23" ns0:compileSdkVersionCodename="6.0-2438415" ns0:installLocation="auto" package="com.odders.ohshape.pico.neo2" platformBuildVersionCode="30" platformBuildVersionName="11"&gt;
+    &lt;supports-screens ns0:anyDensity="true" ns0:largeScreens="true" ns0:normalScreens="true" ns0:smallScreens="true" ns0:xlargeScreens="true" /&gt;
+    &lt;uses-feature ns0:glEsVersion="0x00030000" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.touchscreen" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch.distinct" ns0:required="false" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_SETTINGS" /&gt;
+    &lt;uses-permission ns0:name="android.permission.REORDER_TASKS" /&gt;
+    &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.INTERNET" /&gt;
+    &lt;uses-permission ns0:name="android.permission.ACCESS_NETWORK_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.ACCESS_WIFI_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.RECORD_AUDIO" /&gt;
+    &lt;uses-permission ns0:name="android.permission.MODIFY_AUDIO_SETTINGS" /&gt;
+    &lt;uses-permission ns0:name="android.permission.BLUETOOTH" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.microphone" ns0:required="false" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_EXTERNAL_STORAGE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.READ_EXTERNAL_STORAGE" /&gt;
+    &lt;application ns0:allowBackup="true" ns0:icon="@mipmap/app_icon" ns0:label="@string/app_name" ns0:requestLegacyExternalStorage="true" ns0:supportsRtl="true" ns0:usesCleartextTraffic="true"&gt;
+        &lt;activity ns0:configChanges="density|fontScale|keyboard|keyboardHidden|layoutDirection|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:launchMode="singleTask" ns0:name="com.unity3d.player.UnityPlayerActivity" ns0:screenOrientation="landscape" ns0:theme="@style/UnityThemeSelector"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="android.intent.action.MAIN" /&gt;
+                &lt;category ns0:name="android.intent.category.LAUNCHER" /&gt;
+            &lt;/intent-filter&gt;
+            &lt;meta-data ns0:name="unityplayer.UnityActivity" ns0:value="true" /&gt;
+            &lt;meta-data ns0:name="android.notch_support" ns0:value="true" /&gt;
+            &lt;meta-data ns0:name="android.notch_support" ns0:value="true" /&gt;
+        &lt;/activity&gt;
+        &lt;meta-data ns0:name="unity.splash-mode" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="unity.splash-enable" ns0:value="true" /&gt;
+        &lt;meta-data ns0:name="notch.config" ns0:value="portrait|landscape" /&gt;
+        &lt;meta-data ns0:name="unity.build-id" ns0:value="0ea0d07a-9d72-4946-8645-e39c1750c105" /&gt;
+        &lt;meta-data ns0:name="pvr.app.type" ns0:value="vr" /&gt;
+        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="XR Platform_2.0.4.3" /&gt;
+        &lt;meta-data ns0:name="enable_cpt" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="1" /&gt;
+        &lt;meta-data ns0:name="pico_app_id" ns0:value="83a7cd05349ad5c38f5c8fa53466239b" /&gt;
+        &lt;meta-data ns0:name="pico_app_key" ns0:value="317b35cecd1fc75c3cb3e022deacd002" /&gt;
+        &lt;meta-data ns0:name="pico_scope" ns0:value="get_user_info" /&gt;
+        &lt;meta-data ns0:name="pico_pay_key" ns0:value="ae7b982818ff89a2f7b0fed2ffb4c048" /&gt;
+        &lt;meta-data ns0:name="pico_app_id_foreign" ns0:value="83a7cd05349ad5c38f5c8fa53466239b" /&gt;
+        &lt;meta-data ns0:name="pico_app_key_foreign" ns0:value="317b35cecd1fc75c3cb3e022deacd002" /&gt;
+        &lt;meta-data ns0:name="pico_scope_foreign" ns0:value="get_user_info" /&gt;
+        &lt;meta-data ns0:name="pico_pay_key_foreign" ns0:value="ae7b982818ff89a2f7b0fed2ffb4c048" /&gt;
+        &lt;activity ns0:excludeFromRecents="true" ns0:exported="true" ns0:launchMode="singleTask" ns0:name="com.pico.loginpaysdk.auth.TransferStationActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="com.pico.loginpaysdk.intent.action.AuthCallback" /&gt;
+                &lt;category ns0:name="android.intent.category.DEFAULT" /&gt;
+            &lt;/intent-filter&gt;
+        &lt;/activity&gt;
+        &lt;activity ns0:name="com.yasirkula.unity.NativeShareCustomShareDialogActivity" ns0:theme="@style/Theme.NativeShareTransparent" /&gt;
+        &lt;provider ns0:authorities="com.odders.ohshape.pico.neo2.NativeShareContentProvider" ns0:exported="false" ns0:grantUriPermissions="true" ns0:name="com.yasirkula.unity.NativeShareContentProvider" /&gt;
+        &lt;activity ns0:configChanges="fontScale|keyboard|keyboardHidden|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="true" ns0:name="com.unity3d.services.ads.adunit.AdUnitActivity" ns0:theme="@android:style/Theme.NoTitleBar.Fullscreen" /&gt;
+        &lt;activity ns0:configChanges="fontScale|keyboard|keyboardHidden|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="true" ns0:name="com.unity3d.services.ads.adunit.AdUnitTransparentActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar.Fullscreen" /&gt;
+        &lt;activity ns0:configChanges="fontScale|keyboard|keyboardHidden|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:name="com.unity3d.services.ads.adunit.AdUnitTransparentSoftwareActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar.Fullscreen" /&gt;
+        &lt;activity ns0:configChanges="fontScale|keyboard|keyboardHidden|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:name="com.unity3d.services.ads.adunit.AdUnitSoftwareActivity" ns0:theme="@android:style/Theme.NoTitleBar.Fullscreen" /&gt;
+    &lt;/application&gt;
+&lt;/manifest&gt;</t>
+  </si>
+  <si>
     <t>OpenBrush（绘画，英文）_2.0.0</t>
   </si>
   <si>
     <t>Open Brush 汉化中文版，支持Quest一体机、Pico3、Pico4一体机设备  
 《Tilt Brush》倾斜的刷子(画画神器) 升级版，和谷歌VR绘画一样，功能还多了些，比如可以开启透视功能实现MR混合现实绘画。</t>
+  </si>
+  <si>
+    <t>Based on the permissions and features mentioned, the following sensitive permissions and features should not be requested:
+Sensitive Permissions:
+- No sensitive permissions are mentioned in the question.
+Sensitive Features:
+- No sensitive features are mentioned in the question.</t>
+  </si>
+  <si>
+    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="29" ns0:compileSdkVersionCodename="10" ns0:installLocation="auto" package="com.icosa.openbrush" platformBuildVersionCode="29" platformBuildVersionName="10"&gt;
+    &lt;supports-screens ns0:anyDensity="true" ns0:largeScreens="true" ns0:normalScreens="true" ns0:smallScreens="true" ns0:xlargeScreens="true" /&gt;
+    &lt;uses-feature ns0:glEsVersion="0x00030001" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.opengles.aep" /&gt;
+    &lt;uses-permission ns0:name="android.permission.INTERNET" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_EXTERNAL_STORAGE" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.touchscreen" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch.distinct" ns0:required="false" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_SETTINGS" /&gt;
+    &lt;application ns0:allowBackup="false" ns0:extractNativeLibs="true" ns0:icon="@mipmap/app_icon" ns0:label="@string/app_name" ns0:requestLegacyExternalStorage="true"&gt;
+        &lt;activity ns0:configChanges="density|fontScale|keyboard|keyboardHidden|layoutDirection|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:launchMode="singleTask" ns0:name="com.unity3d.player.UnityPlayerActivity" ns0:resizeableActivity="false" ns0:screenOrientation="landscape"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="android.intent.action.MAIN" /&gt;
+                &lt;category ns0:name="android.intent.category.LAUNCHER" /&gt;
+            &lt;/intent-filter&gt;
+        &lt;/activity&gt;
+        &lt;meta-data ns0:name="unityplayer.SkipPermissionsDialog" ns0:value="false" /&gt;
+        &lt;meta-data ns0:name="unity.splash-mode" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="unity.splash-enable" ns0:value="true" /&gt;
+        &lt;meta-data ns0:name="unity.launch-fullscreen" ns0:value="true" /&gt;
+        &lt;meta-data ns0:name="unity.allow-resizable-window" ns0:value="false" /&gt;
+        &lt;meta-data ns0:name="pvr.app.type" ns0:value="vr" /&gt;
+        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="XR Platform_2.1.2.2" /&gt;
+        &lt;meta-data ns0:name="enable_cpt" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="handtracking" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="rendering_mode" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="display_rate" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="color_Space" ns0:value="1" /&gt;
+        &lt;meta-data ns0:name="MRCsupport" ns0:value="0" /&gt;
+    &lt;/application&gt;
+&lt;/manifest&gt;</t>
+  </si>
+  <si>
+    <t>Squingle_2.0.9(1)</t>
+  </si>
+  <si>
+    <t>单人游戏，而且需要使用摄像头来与外界互动。
+【名称】：Squingle VR
+【类型】：解密/益智
+【平台】：Oculus Quest &amp; 二代
+【联机】：单人离线
+【大小】：360MB
+【刷新】：90Hz
+【语言】：英文
+【说明】：
+在时间之前只有 Squingle – 她需要你的帮助来创造宇宙！
+引导旋转球体穿过 100 个手工制作的、扭曲和旋转的彩虹色迷宫，然后与自己的幽灵赛跑！
+通过不断变化的音乐音景和“属于自己的迷幻视觉效果”解决巧妙的难题。你会发现 Squinle 的意思吗？
+“将成为VR历史上的经典！”
+“充满风格，独特而令人敬畏”
+“玩起来超级满足”
+“客观上是 Quest 2 上一些最好的图形和声音”</t>
+  </si>
+  <si>
+    <t>Based on the description and the permissions and features mentioned, the following sensitive permissions and features should not be requested:
+Sensitive permissions:
+- android.permission.WRITE_SETTINGS: This permission allows the app to modify system settings. It is not necessary for the functionality described in the game description.
+Sensitive features:
+- android.hardware.camera: The game description mentions that the camera is used for interacting with the outside world. However, the use of the camera is not explicitly required for the gameplay itself, so this feature may not be necessary.</t>
   </si>
   <si>
     <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="30" ns0:compileSdkVersionCodename="11" ns0:installLocation="auto" package="com.SquingleStudios.Squingle" platformBuildVersionCode="30" platformBuildVersionName="11"&gt;
@@ -1425,7 +1220,13 @@
 &lt;/manifest&gt;</t>
   </si>
   <si>
-    <t>Squingle_2.0.9(1)</t>
+    <t>&lt;uses-permission ns0:name="android.permission.CAMERA" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.camera" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.camera.autofocus" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.camera.front" ns0:required="false" /&gt;
+    &lt;uses-permission ns0:name="android.permission.RECORD_AUDIO" /&gt;
+    &lt;uses-permission ns0:name="android.permission.MODIFY_AUDIO_SETTINGS" /&gt;
+ &lt;uses-feature ns0:name="android.hardware.microphone" ns0:required="false" /&gt;</t>
   </si>
   <si>
     <t>VR驾校_3.97</t>
@@ -1437,12 +1238,12 @@
 什么是车感？就是在车内对外部环境的距离感知，有的人距离感强，很快就能练成，有的人距离感弱，需要更长的时间；大多数人对距离不敏感，但是对色彩却很敏感，根据这一特点我们设计了一整套动态色彩练车系统：红色表示当前车距离“标线的标准位置”差距很大；绿色表示当前车距离“标线的标准位置”相差无几，是下一步操作时机。 当前车的位置越标准越绿，越不标准越红。</t>
   </si>
   <si>
-    <t>Based on the permissions and features mentioned in the question, the sensitive permissions and features that should not be requested are:
-Permissions:
-- android.permission.ACCESS_FINE_LOCATION (Not relevant to the game description)
-- android.permission.WRITE_SETTINGS (Not relevant to the game description)
-Features:
-- android.hardware.location.gps (Not required according to the game description)</t>
+    <t>Based on the provided information, the sensitive permissions and features that should not be requested are:
+Sensitive Permissions:
+- android.permission.ACCESS_FINE_LOCATION: This permission is not required for the functionality of the game description.
+Sensitive Features:
+- android.hardware.location.gps: This feature is not required for the functionality of the game description.
+- android.hardware.location: This feature is not required for the functionality of the game description.</t>
   </si>
   <si>
     <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="23" ns0:compileSdkVersionCodename="6.0-2438415" ns0:installLocation="auto" package="com.HFNK.car.pico" platformBuildVersionCode="30" platformBuildVersionName="11"&gt;
@@ -1501,14 +1302,6 @@
 通过您最喜欢的锻炼进行热身或训练。
 如果您喜欢挑战，请选择最激烈的模式，一定可以保证值得一做，这也很有趣！
 除此之外，借助X-BOOSTER，您可以创建自己的训练并按照自己的步调前进！</t>
-  </si>
-  <si>
-    <t>Based on the permissions and features mentioned, the following sensitive permissions and features should not be requested:
-Sensitive Permissions:
-- android.permission.WRITE_EXTERNAL_STORAGE: This permission allows the app to write to external storage, which can potentially access and modify user's personal data. It is not necessary for a music rhythm game and can be considered intrusive.
-Sensitive Features:
-None of the features mentioned are considered sensitive.
-Therefore, the app should not request the WRITE_EXTERNAL_STORAGE permission.</t>
   </si>
   <si>
     <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="30" ns0:compileSdkVersionCodename="11" ns0:installLocation="auto" package="com.nivision.xbooster" platformBuildVersionCode="30" platformBuildVersionName="11"&gt;
@@ -1554,19 +1347,6 @@
 在那里，人们必须在有限的时间内破解所有的机关谜题，才能逃出这个奇怪的空间，否则就会永远留在那里，变成娃娃一直陪着她玩……
 游戏画面和音效方面很不错，对于恐怖氛围的营造比较到位，关卡中的解谜问题也很有趣味性和益智性。但游戏没有多人模式，流程不长的线性故事关卡也是固定的，对这样一款游戏来说略显遗憾。
 《不说话的娃娃》上新首周享受7折优惠，喜欢恐怖解谜类游戏的用户可以趁此机会入手，体验一下不一样的密室逃脱~</t>
-  </si>
-  <si>
-    <t>Based on the permissions and features mentioned, the following sensitive permissions and features should not be requested:
-Sensitive Permissions:
-- android.permission.RECORD_AUDIO
-- android.permission.MODIFY_AUDIO_SETTINGS
-- android.permission.WRITE_EXTERNAL_STORAGE
-- android.permission.READ_EXTERNAL_STORAGE
-- android.permission.INJECT_EVENTS
-- android.permission.WRITE_SETTINGS
-- android.permission.CHANGE_CONFIGURATION
-Sensitive Features:
-- android.hardware.microphone (required="false")</t>
   </si>
   <si>
     <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="28" ns0:compileSdkVersionCodename="9" ns0:installLocation="auto" package="com.GoodNet.TheSilentDoll" platformBuildVersionCode="28" platformBuildVersionName="9"&gt;
@@ -1654,26 +1434,12 @@
 &lt;/manifest&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">  &lt;uses-permission ns0:name="android.permission.RECORD_AUDIO" /&gt;
-    &lt;uses-permission ns0:name="android.permission.MODIFY_AUDIO_SETTINGS" /&gt;</t>
-  </si>
-  <si>
     <t>创世神_Deisim_1.37</t>
   </si>
   <si>
     <t>开疆拓土、呼风唤雨，只需要动动手指
 在《Deisim VR》中，玩家扮演的是造物者，这个身份玩家主要能做三件事，创造、维护和破坏。
 玩家按X呼出菜单，可以在一片没有任何限制的空间中，选择平原、森林、樱花林、水面、雪地、沙漠、荒漠、火山等等各种地形进行布置。同时也可以在地形之上放置动物、矿物等等。</t>
-  </si>
-  <si>
-    <t>Based on the given permissions and features mentioned in the question, the sensitive permissions and features that should not be requested are:
-Sensitive Permissions:
-- android.permission.REORDER_TASKS
-Sensitive Features:
-- android.hardware.vulkan.version (with required="false")
-- android.hardware.touchscreen (with required="false")
-- android.hardware.touchscreen.multitouch (with required="false")
-- android.hardware.touchscreen.multitouch.distinct (with required="false")</t>
   </si>
   <si>
     <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="23" ns0:compileSdkVersionCodename="6.0-2438415" ns0:installLocation="auto" package="com.MyronSoftware.Deisim" platformBuildVersionCode="30" platformBuildVersionName="11"&gt;
@@ -1728,17 +1494,6 @@
   </si>
   <si>
     <t>《忍者传奇Ninjia Legends》是一款快节奏的格斗游戏。是笔者目前接触过的一体机VR游戏里，消耗卡路里效果最好的一款游戏，画面逼真，游戏过程充满紧张感，就像是自己和一群忍者进行近身格斗一样，对战boss的感觉就像真人格斗对打，游玩过程中，要有充分的体力，打出有力道的攻击，同时，身法要灵活，多运用移动和转身进行闪避和攻击多方向来袭的敌人。游戏中，可选择双刀，长刀，大刀，弓箭，利爪，圈套，权杖，长短刀作为武器，还可选择各种炫酷特技。这款游戏属于一体机游戏里比较早的游戏了，但笔者感觉可玩性还是比较高的</t>
-  </si>
-  <si>
-    <t>Based on the game description and the mentioned permissions and features, the sensitive permissions and features that should not be requested are as follows:
-Sensitive Permissions to Avoid:
-1. android.permission.WRITE_SETTINGS
-2. android.permission.CHANGE_CONFIGURATION
-3. android.permission.INJECT_EVENTS
-4. android.permission.REORDER_TASKS
-Reasoning: These permissions are potentially risky as they allow the app to modify system settings, change device configurations, inject events into the input stream, and reorder tasks, respectively. These permissions can be misused to interfere with the device's normal operations or compromise user privacy and security.
-Sensitive Features to Avoid:
-None of the mentioned features are sensitive.</t>
   </si>
   <si>
     <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="29" ns0:compileSdkVersionCodename="10" ns0:installLocation="auto" package="com.coinflip.ninja.ch" platformBuildVersionCode="11" platformBuildVersionName="1.0.11"&gt;
@@ -1829,13 +1584,6 @@
     <t>作为一款模拟攀岩的VR游戏，《急速攀岩》主打手部攀爬机制，玩家在攀岩的过程中需要借助头手6DoF手柄来控制游戏中的角色的双手，通过双手不断交替攀爬进行移动，同时还不忘一直仰头找寻下一个支点，因此，一场游戏下来玩家的肩颈会得到充分地锻炼。</t>
   </si>
   <si>
-    <t>Based on the information provided, the sensitive permissions and features that should not be requested are:
-Sensitive Permissions:
-1. android.permission.REORDER_TASKS - This permission allows the app to change the order of tasks or activities on the device. It is not necessary for the described game and could potentially be misused.
-Sensitive Features:
-None of the mentioned features are considered sensitive.</t>
-  </si>
-  <si>
     <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="29" ns0:compileSdkVersionCodename="10" ns0:installLocation="auto" package="com.mirage.RocktoTop" platformBuildVersionCode="29" platformBuildVersionName="10"&gt;
     &lt;supports-screens ns0:anyDensity="true" ns0:largeScreens="true" ns0:normalScreens="true" ns0:smallScreens="true" ns0:xlargeScreens="true" /&gt;
     &lt;uses-permission ns0:name="android.permission.ACCESS_NETWORK_STATE" /&gt;
@@ -1886,17 +1634,6 @@
   </si>
   <si>
     <t>《愤怒的小鸟VR》游戏目标非常简单：我们的对手是一群洋洋得意目中无人的绿色小猪，盘踞在我们面前的空地上并用各种或一碰即碎或坚不可摧的材料搭建成各种摇摇欲坠的奇怪“城寨”。我们的任务就是仔细观察寻找这些“城寨”的结构弱点，并把手边的小鸟（数量非常有限）用“弹弓”发射出去，准确命中结构弱点从而让“城寨”毁于一旦。</t>
-  </si>
-  <si>
-    <t>Based on the provided information, the following sensitive permissions and features should not be requested:
-Permissions:
-1. android.permission.WRITE_SETTINGS
-2. android.permission.CHANGE_CONFIGURATION
-3. android.permission.INJECT_EVENTS
-4. com.android.vending.BILLING
-5. android.permission.REORDER_TASKS
-Features:
-None of the mentioned features are sensitive and can be requested.</t>
   </si>
   <si>
     <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="29" ns0:compileSdkVersionCodename="10" ns0:installLocation="auto" package="com.resolutiongames.abvriop.piconeo" platformBuildVersionCode="29" platformBuildVersionName="10"&gt;
@@ -2038,29 +1775,6 @@
 &lt;/manifest&gt;</t>
   </si>
   <si>
-    <t>战机激战太平洋_WarplanesBattlesoverPacific_1.1.2.1</t>
-  </si>
-  <si>
-    <t>战机：太平洋战争开启了航空史的下一个篇章。成为第二次世界大战的飞行员，参加对抗日本帝国的战役。《Warplanes: WW1 Fighters》的续集将格斗提升到了一个新的水平。
-逼真的图形和直观的控件增强了游戏体验。新的飞行模型将让你感受到最受欢迎的美国和日本飞机的动力、速度和操控性。第一次世界大战和第二次世界大战之间的技术飞跃使航空成为军队的主要分支，并永远改变了战争。。。
-虚拟现实中的二战体验
-● 带领美国在单人战役中战胜日本。
-● 玩经典的PvP多人模式来对抗来自世界各地的玩家。
-● 和你身边的朋友一起享受合作任务的乐趣。
-● 控制10架在太平洋上空作战的最具标志性的飞机。
-● 由于有3个难度级别，可以根据自己的喜好调整游戏。</t>
-  </si>
-  <si>
-    <t>Based on the permissions and features mentioned, the sensitive permissions and features that should not be requested are:
-Sensitive permissions:
-1. android.permission.RECORD_AUDIO - This permission is not necessary for the described game and may be considered intrusive for users.
-2. android.permission.WRITE_SETTINGS - This permission allows the app to modify system settings, which is not required for the game functionality.
-Sensitive features:
-1. android.hardware.vr.headtracking - This feature indicates the game supports virtual reality and may require additional hardware, which may not be necessary for all users.
-2. android.hardware.microphone - This feature indicates the game utilizes the microphone, which may be considered intrusive for users and not necessary for the described gameplay.
-It's important for developers to only request permissions and features that are necessary for the functionality of their app and to respect user privacy.</t>
-  </si>
-  <si>
     <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="29" ns0:compileSdkVersionCodename="10" ns0:installLocation="auto" package="com.HomeNetGames.WW2VR" platformBuildVersionCode="29" platformBuildVersionName="10"&gt;
     &lt;supports-screens ns0:anyDensity="true" ns0:largeScreens="true" ns0:normalScreens="true" ns0:smallScreens="true" ns0:xlargeScreens="true" /&gt;
     &lt;uses-feature ns0:name="android.hardware.vr.headtracking" ns0:required="true" ns0:version="1" /&gt;
@@ -2106,28 +1820,6 @@
         &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="1" /&gt;
     &lt;/application&gt;
 &lt;/manifest&gt;</t>
-  </si>
-  <si>
-    <t>掘金者_CaveDigger_2.12</t>
-  </si>
-  <si>
-    <t>Cave Digger」游戏背景设定在一个充斥着黑色幽默元素的另类西方世界，玩家将扮演一名掘金者深入地下矿井挖掘宝藏，并不断升级或解锁挖掘工具以提高挖掘效率；续作「Cave Digger 2：Dig Harder」沿用了「Cave Digger」背景，并添加了包括4人合作模式和更豪华柴油朋克世界在内的更多内容，玩家将继续在游戏中挖掘宝藏以及探究隐藏秘密。</t>
-  </si>
-  <si>
-    <t>Based on the description and the information provided, the following sensitive permissions and features should not be requested:
-Sensitive permissions:
-1. android.permission.RECORD_AUDIO
-2. android.permission.MODIFY_AUDIO_SETTINGS
-3. android.permission.WRITE_EXTERNAL_STORAGE
-4. android.permission.WRITE_SETTINGS
-5. android.permission.MODIFY_AUDIO_SETTINGS
-6. android.permission.REORDER_TASKS
-7. android.permission.READ_EXTERNAL_STORAGE
-Sensitive features:
-1. android.hardware.microphone (required="false")
-2. android.hardware.touchscreen (required="false")
-3. android.hardware.touchscreen.multitouch (required="false")
-4. android.hardware.touchscreen.multitouch.distinct (required="false")</t>
   </si>
   <si>
     <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="30" ns0:compileSdkVersionCodename="11" ns0:installLocation="auto" package="com.mekiwi.cavedigger" platformBuildVersionCode="30" platformBuildVersionName="11"&gt;
@@ -2814,13 +2506,60 @@
     <t>https://www.quest3game.com/picogame/%E9%BB%98%E8%80%85_Sairento_1.9.0.apk</t>
   </si>
   <si>
-    <t>改进策略：
-1.添加单机游戏/联机游戏/
-2.使用···分开xml文件
-3.双重提问，先解析xml文件，后提问
-4.删除冗余的规则，尽量简洁
-仍存在的问题：
-无法根据游戏是否联机判断是否需要录音权限。</t>
+    <t>Based on the information provided, the sensitive permissions and features that should not be requested are:
+Permissions:
+- android.permission.INJECT_EVENTS (this permission can be used for malicious purposes)
+- android.permission.RECORD_AUDIO (this permission is not necessary for the game's functionality)
+- android.permission.MODIFY_AUDIO_SETTINGS (this permission is not necessary for the game's functionality)
+- android.permission.REORDER_TASKS (this permission is not necessary for the game's functionality)
+Features:
+- android.hardware.vr.headtracking (this feature is required but may not be supported on all devices, so the game should handle this gracefully and provide alternative gameplay options for devices that do not support VR headtracking)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Based on the given information, the following sensitive permissions and features should not be requested:
+Permissions: 
+- android.permission.WRITE_SETTINGS (No need to manage system settings for this game)
+- android.permission.WRITE_EXTERNAL_STORAGE (No need to store data in external storage for this game)
+Features: 
+- android.hardware.touchscreen (Not explicitly required for the game)
+- android.hardware.touchscreen.multitouch (Not explicitly required for the game)
+- android.hardware.touchscreen.multitouch.distinct (Not explicitly required for the game)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;uses-permission ns0:name="android.permission.RECORD_AUDIO" /&gt;
+    &lt;uses-permission ns0:name="android.permission.MODIFY_AUDIO_SETTINGS" /&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Based on the permissions mentioned in the question and the given game description, the sensitive permissions that should not be requested are:
+- android.permission.WRITE_SETTINGS
+- android.permission.REORDER_TASKS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Based on the given information, the sensitive permissions and features that should not be requested are:
+- android.permission.INJECT_EVENTS: This permission allows the app to inject user events into the event stream. It can be used for malicious purposes and should not be requested unless absolutely necessary.
+- android.permission.REORDER_TASKS: This permission allows the app to change the order of tasks on the device. It is not necessary for the described game and should not be requested.
+- android.hardware.touchscreen.multitouch: This feature is not required for the game and should not be requested.
+Note: The given description does not provide enough information to determine if any other permissions or features should not be requested.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Based on the permissions and features mentioned, the sensitive permissions and features that should not be requested for this game are:
+- android.permission.REORDER_TASKS
+- android.permission.READ_EXTERNAL_STORAGE
+- android.permission.WRITE_EXTERNAL_STORAGE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Based on the provided information, the sensitive permissions and features that should not be requested are:
+1. android.permission.WRITE: This permission allows the app to modify/delete data on the device's storage. It is not necessary for the described game and could potentially be used for malicious purposes.
+Other permissions mentioned in the question do not seem to be sensitive and may be required for the game's functionality:
+1. android.permission.INTERNET: This permission is required for the game to access the internet and communicate with game servers for online features, updates, or advertisements.
+2. android.permission.ACCESS_NETWORK_STATE: This permission is used to check the network connectivity status of the device, which can be useful for determining if the game can access online features.
+3. android.permission.VIBRATE: This permission allows the game to vibrate the device as part of the gameplay experience.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2829,156 +2568,207 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Based on the permissions and features mentioned in the question, the sensitive permissions and features that should not be requested are:
-- android.permission.RECORD_AUDIO: This permission is not necessary for a World War I flying shooter game.
-- android.permission.ACCESS_WIFI_STATE: This permission is not necessary for a flying shooter game.
-- android.permission.ACCESS_NETWORK_STATE: This permission is not necessary for a flying shooter game.
-- android.permission.WRITE_EXTERNAL_STORAGE: This permission is not necessary for a flying shooter game.
-- android.permission.BLUETOOTH: This permission is not necessary for a flying shooter game.
-- android.permission.WRITE_SETTINGS: This permission is not necessary for a flying shooter game.
-- android.permission.READ_EXTERNAL_STORAGE: This permission is not necessary for a flying shooter game.
-- android.permission.BLUETOOTH_ADMIN: This permission is not necessary for a flying shooter game.
-- android.hardware.vr.headtracking: This feature is not necessary for a flying shooter game.
-- android.hardware.microphone: This feature is not necessary for a flying shooter game.
-- android.hardware.sensor.accelerometer: This feature is not necessary for a flying shooter game.
-- android.hardware.touchscreen: This feature is necessary for a flying shooter game.
-- android.hardware.touchscreen.multitouch: This feature is necessary for a flying shooter game.
-- android.hardware.touchscreen.multitouch.distinct: This feature is necessary for a flying shooter game.
-- oculus.software.overlay_keyboard: This feature is not necessary for a flying shooter game.</t>
+    <t>Based on the permissions and features mentioned, the sensitive permissions and features that should not be requested are:
+Sensitive permissions:
+- android.permission.RECORD_AUDIO (It is not necessary for a flight shooting game and may violate user privacy)
+- android.permission.WRITE_EXTERNAL_STORAGE (It is not necessary for a flight shooting game and may access personal files)
+- android.permission.READ_EXTERNAL_STORAGE (It is not necessary for a flight shooting game and may access personal files)
+Sensitive features:
+- android.hardware.microphone (Not required for a flight shooting game and may violate user privacy)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Based on the permissions and features mentioned in the question, the sensitive permissions and features that should not be requested are:
+    <t>Based on the provided information, the sensitive permissions and features that should not be requested are:
+Permissions:
+- android.permission.RECORD_AUDIO: This permission is not required for the game description provided.
+- android.permission.ACCESS_WIFI_STATE: This permission is not required for the game description provided.
+- android.permission.WRITE_SETTINGS: This permission is not required for the game description provided.
+Features:
+- android.hardware.microphone: This feature is not required for the game description provided.
+- android.hardware.sensor.accelerometer: This feature is not required for the game description provided.
+- android.hardware.touchscreen.multitouch: This feature is not required for the game description provided.
+- android.hardware.touchscreen.multitouch.distinct: This feature is not required for the game description provided.
+- oculus.software.overlay_keyboard: This feature is not required for the game description provided.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Based on the given information, the following sensitive permissions and features should not be requested:
 Sensitive Permissions:
-1. android.permission.RECORD_AUDIO - This permission allows the app to record audio, which may be a privacy concern for users.
+- android.permission.RECORD_AUDIO: This permission is not required for the game.
+- android.permission.MODIFY_AUDIO_SETTINGS: This permission is not required for the game.
+- android.permission.WRITE_EXTERNAL_STORAGE: This permission is not required for the game.
+- android.permission.WRITE_SETTINGS: This permission is not required for the game.
+- android.permission.REORDER_TASKS: This permission is not required for the game.
+- android.permission.READ_EXTERNAL_STORAGE: This permission is not required for the game.
 Sensitive Features:
-1. android.hardware.microphone (required=false) - This feature indicates that the app does not require access to the device's microphone, which is a sensitive feature for privacy reasons.</t>
+- android.hardware.microphone: This feature is not required for the game.
+- android.hardware.touchscreen.multitouch: This feature is not required for the game.
+- android.hardware.touchscreen.multitouch.distinct: This feature is not required for the game.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Based on the given permissions and features, the sensitive permissions that should not be requested for the game "启示骑士" are:
-- android.permission.INTERNET
+    <t>掘金者_CaveDigger_2.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cave Digger」游戏背景设定在一个充斥着黑色幽默元素的另类西方世界，玩家将扮演一名掘金者深入地下矿井挖掘宝藏，并不断升级或解锁挖掘工具以提高挖掘效率；续作「Cave Digger 2：Dig Harder」沿用了「Cave Digger」背景，并添加了包括4人合作模式和更豪华柴油朋克世界在内的更多内容，玩家将继续在游戏中挖掘宝藏以及探究隐藏秘密。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>战机激战太平洋_WarplanesBattlesoverPacific_1.1.2.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>战机：太平洋战争开启了航空史的下一个篇章。成为第二次世界大战的飞行员，参加对抗日本帝国的战役。《Warplanes: WW1 Fighters》的续集将格斗提升到了一个新的水平。逼真的图形和直观的控件增强了游戏体验。新的飞行模型将让你感受到最受欢迎的美国和日本飞机的动力、速度和操控性。第一次世界大战和第二次世界大战之间的技术飞跃使航空成为军队的主要分支，并永远改变了战争。。。虚拟现实中的二战体验● 带领美国在单人战役中战胜日本。● 玩经典的PvP多人模式来对抗来自世界各地的玩家。● 和你身边的朋友一起享受合作任务的乐趣。● 控制10架在太平洋上空作战的最具标志性的飞机。● 由于有3个难度级别，可以根据自己的喜好调整游戏。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Based on the provided information, the sensitive permissions and features that should not be requested are:
+Permissions:
+- android.permission.SYSTEM_ALERT_WINDOW
+- android.permission.WRITE_MEDIA_STORAGE
+- android.permission.WRITE_SECURE_SETTINGS
+- android.permission.INJECT_EVENTS
+- android.permission.DEVICE_POWER
+- android.permission.RECORD_AUDIO
+- android.permission.MODIFY_AUDIO_SETTINGS
+- android.permission.REORDER_TASKS
+Features:
+- android.hardware.microphone
+- android.hardware.touchscreen.multitouch
+- android.hardware.touchscreen.multitouch.distinct</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Based on the permissions and features mentioned, the sensitive permissions and features that should not be requested are:
+- android.permission.WRITE_EXTERNAL_STORAGE: This permission allows the app to write to external storage, which may not be necessary for the game.
+- com.android.vending.CHECK_LICENSE: This permission is specific to Google Play and is used to check the licensing status of the app. It is not necessary for the game.
+- android.permission.READ_EXTERNAL_STORAGE: This permission allows the app to read from external storage, which may not be necessary for the game.
+- android.permission.WRITE_SETTINGS: This permission allows the app to modify system settings, which may not be necessary for the game.
+- android.permission.CHANGE_CONFIGURATION: This permission allows the app to change the device's configuration, which may not be necessary for the game.
+- android.permission.INJECT_EVENTS: This permission allows the app to inject events into the input system, which could potentially be used for malicious purposes and is not necessary for the game.
+As for the features mentioned, the game only utilizes the android.hardware.touchscreen feature, which is expected for a game and does not raise any concerns.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="30" ns0:compileSdkVersionCodename="11" ns0:installLocation="auto" package="com.vrm.aporiderNeo2" platformBuildVersionCode="69" platformBuildVersionName="1.7.8"&gt;
+    &lt;uses-feature ns0:glEsVersion="0x00030001" ns0:required="true" /&gt;
+    &lt;uses-permission ns0:name="android.permission.INTERNET" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_EXTERNAL_STORAGE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.ACCESS_NETWORK_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WAKE_LOCK" /&gt;
+    &lt;uses-permission ns0:name="com.android.vending.CHECK_LICENSE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.ACCESS_WIFI_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.MODIFY_AUDIO_SETTINGS" /&gt;
+    &lt;uses-permission ns0:name="android.permission.VIBRATE" /&gt;
+    &lt;supports-gl-texture ns0:name="GL_KHR_texture_compression_astc_ldr" /&gt;
+    &lt;uses-permission ns0:name="android.permission.READ_EXTERNAL_STORAGE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_SETTINGS" /&gt;
+    &lt;uses-permission ns0:name="android.permission.CHANGE_CONFIGURATION" /&gt;
+    &lt;uses-permission ns0:name="android.permission.BLUETOOTH" /&gt;
+    &lt;uses-permission ns0:name="android.permission.BLUETOOTH_ADMIN" /&gt;
+    &lt;uses-permission ns0:name="android.permission.INJECT_EVENTS" /&gt;
+    &lt;application ns0:debuggable="true" ns0:hardwareAccelerated="false" ns0:hasCode="true" ns0:icon="@drawable/icon" ns0:label="@string/app_name" ns0:name="com.epicgames.ue4.GameApplication" ns0:requestLegacyExternalStorage="true"&gt;
+        &lt;activity ns0:configChanges="keyboard|keyboardHidden|navigation|orientation|screenSize" ns0:debuggable="true" ns0:hardwareAccelerated="false" ns0:label="@string/app_name" ns0:launchMode="singleTask" ns0:name="com.epicgames.ue4.SplashActivity" ns0:screenOrientation="landscape" ns0:theme="@style/UE4SplashTheme"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="android.intent.action.MAIN" /&gt;
+                &lt;category ns0:name="android.intent.category.LAUNCHER" /&gt;
+            &lt;/intent-filter&gt;
+        &lt;/activity&gt;
+        &lt;activity ns0:configChanges="keyboard|keyboardHidden|navigation|orientation|screenSize" ns0:debuggable="true" ns0:hardwareAccelerated="false" ns0:label="@string/app_name" ns0:launchMode="singleTask" ns0:name="com.epicgames.ue4.GameActivity" ns0:resizeableActivity="false" ns0:screenOrientation="landscape" ns0:theme="@style/UE4SplashTheme"&gt;
+            &lt;meta-data ns0:name="android.app.lib_name" ns0:value="UE4" /&gt;
+        &lt;/activity&gt;
+        &lt;activity ns0:configChanges="keyboard|keyboardHidden|navigation|orientation|screenSize" ns0:hardwareAccelerated="false" ns0:name="com.vrm.aporiderNeo2.DownloaderActivity" ns0:screenOrientation="landscape" ns0:theme="@style/UE4SplashTheme" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.EngineVersion" ns0:value="4.24.3" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.EngineBranch" ns0:value="++UE4+Release-4.24" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.ProjectVersion" ns0:value="2.5.1" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.DepthBufferPreference" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bPackageDataInsideApk" ns0:value="true" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bVerifyOBBOnStartUp" ns0:value="false" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bShouldHideUI" ns0:value="true" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.ProjectName" ns0:value="ApocalypseRider" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.AppType" ns0:value="" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bHasOBBFiles" ns0:value="true" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.BuildConfiguration" ns0:value="Development" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.CookedFlavors" ns0:value="ASTC" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bValidateTextureFormats" ns0:value="true" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bUseExternalFilesDir" ns0:value="false" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bPublicLogFiles" ns0:value="false" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bUseDisplayCutout" ns0:value="false" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bAllowIMU" ns0:value="true" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.bSupportsVulkan" ns0:value="false" /&gt;
+        &lt;meta-data ns0:name="com.epicgames.ue4.GameActivity.StartupPermissions" ns0:value="" /&gt;
+        &lt;meta-data ns0:name="com.google.android.gms.games.APP_ID" ns0:value="@string/app_id" /&gt;
+        &lt;meta-data ns0:name="com.google.android.gms.version" ns0:value="@integer/google_play_services_version" /&gt;
+        &lt;service ns0:name="com.vrm.aporiderNeo2.OBBDownloaderService" /&gt;
+        &lt;receiver ns0:name="com.vrm.aporiderNeo2.AlarmReceiver" /&gt;
+        &lt;receiver ns0:name="com.epicgames.ue4.LocalNotificationReceiver" /&gt;
+        &lt;receiver ns0:exported="true" ns0:name="com.epicgames.ue4.MulticastBroadcastReceiver"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="com.android.vending.INSTALL_REFERRER" /&gt;
+            &lt;/intent-filter&gt;
+        &lt;/receiver&gt;
+        &lt;meta-data ns0:name="android.max_aspect" ns0:value="2100000.0" /&gt;
+        &lt;activity ns0:configChanges="keyboard|keyboardHidden|navigation|orientation|screenSize" ns0:excludeFromRecents="true" ns0:exported="true" ns0:hardwareAccelerated="false" ns0:launchMode="singleTask" ns0:name="com.pico.loginpaysdk.auth.TransferStationActivity" ns0:screenOrientation="landscape" ns0:theme="@android:style/Theme.Translucent.NoTitleBar"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="com.pico.loginpaysdk.intent.action.AuthCallback" /&gt;
+                &lt;category ns0:name="android.intent.category.DEFAULT" /&gt;
+            &lt;/intent-filter&gt;
+        &lt;/activity&gt;
+        &lt;meta-data ns0:name="pico_app_id" ns0:value="6a3e998619ccfdb1ef114145f3ad7224" /&gt;
+        &lt;meta-data ns0:name="pico_app_key" ns0:value="" /&gt;
+        &lt;meta-data ns0:name="pico_scope" ns0:value="get_user_info" /&gt;
+        &lt;meta-data ns0:name="pico_merchant_id" ns0:value="" /&gt;
+        &lt;meta-data ns0:name="pico_pay_key" ns0:value="" /&gt;
+        &lt;meta-data ns0:name="pvr.app.type" ns0:value="vr" /&gt;
+        &lt;meta-data ns0:name="pvr.display.orientation" ns0:value="180" /&gt;
+        &lt;meta-data ns0:name="platform_logo" ns0:value="1" /&gt;
+        &lt;meta-data ns0:name="loadingtextsize" ns0:value="16" /&gt;
+        &lt;meta-data ns0:name="loadingwidth" ns0:value="500" /&gt;
+        &lt;meta-data ns0:name="loadingheight" ns0:value="100" /&gt;
+        &lt;meta-data ns0:name="loadingmarquee" ns0:value="1" /&gt;
+        &lt;meta-data ns0:name="bottommargin" ns0:value="100" /&gt;
+        &lt;meta-data ns0:name="marqueecount" ns0:value="10" /&gt;
+        &lt;meta-data ns0:name="loadingalign" ns0:value="left" /&gt;
+        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="UE4_1.2.5.5" /&gt;
+        &lt;meta-data ns0:name="com.pvr.hmd.trackingmode" ns0:value="6dof" /&gt;
+        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="1" /&gt;
+        &lt;activity ns0:excludeFromRecents="true" ns0:exported="false" ns0:name="com.google.android.gms.auth.api.signin.internal.SignInHubActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar" /&gt;
+        &lt;service ns0:exported="true" ns0:name="com.google.android.gms.auth.api.signin.RevocationBoundService" ns0:permission="com.google.android.gms.auth.api.signin.permission.REVOCATION_NOTIFICATION" /&gt;
+        &lt;provider ns0:authorities="com.vrm.aporiderNeo2.lifecycle-trojan" ns0:exported="false" ns0:multiprocess="true" ns0:name="android.arch.lifecycle.ProcessLifecycleOwnerInitializer" /&gt;
+        &lt;activity ns0:exported="false" ns0:name="com.google.android.gms.common.api.GoogleApiActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar" /&gt;
+    &lt;/application&gt;
+&lt;/manifest&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Based on the game description, the following sensitive permissions and features should not be requested:
+Sensitive permissions: 
 - android.permission.WRITE_EXTERNAL_STORAGE
-- android.permission.READ_EXTERNAL_STORAGE</t>
+- android.permission.WRITE_SETTINGS
+- android.permission.READ_EXTERNAL_STORAGE
+Sensitive features: 
+- None mentioned in the game description</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Based on the permissions and features mentioned in the question, the sensitive permissions and features that should not be requested are:
-1. android.permission.READ_EXTERNAL_STORAGE
-2. android.permission.WRITE_EXTERNAL_STORAGE
-3. android.permission.INJECT_EVENTS
-4. android.permission.RECORD_AUDIO
-5. android.permission.ACCESS_FINE_LOCATION
-6. android.permission.CAMERA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Based on the game description and the mentioned permissions and features, the following sensitive permissions and features should not be requested:
-Sensitive Permissions:
-1. android.permission.WRITE_SETTINGS: This permission grants the app the ability to modify system settings, which is not necessary for a game of this nature.
-2. android.permission.REORDER_TASKS: This permission allows the app to move tasks to the front or back of the task stack, which is unnecessary for a game.
-Sensitive Features:
-None of the features mentioned in the game description indicate a need for sensitive features.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Based on the provided information, the sensitive permissions and features that should not be requested are:
-Sensitive Permissions:
-- android.permission.WRITE_SETTINGS
-- android.permission.REORDER_TASKS
-Sensitive Features:
-- None mentioned in the question.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Based on the permissions and features mentioned and the game description provided, the sensitive permissions and features that should not be requested are:
-1. android.permission.WRITE_EXTERNAL_STORAGE and android.permission.READ_EXTERNAL_STORAGE - These permissions are not mentioned in the game description and are not necessary for the functionality described.
-2. android.permission.INJECT_EVENTS - This permission is not mentioned in the game description and may have potential security implications.
-3. android.permission.RECORD_AUDIO and android.permission.MODIFY_AUDIO_SETTINGS - These permissions are not mentioned in the game description and are not necessary for the functionality described.
-4. android.hardware.microphone - This feature is not mentioned in the game description and may have potential privacy implications.
-5. android.hardware.sensor.accelerometer - This feature is not mentioned in the game description and may not be necessary for the gameplay.
-6. android.hardware.touchscreen.multitouch and android.hardware.touchscreen.multitouch.distinct - These features are not mentioned in the game description and may not be necessary for the gameplay.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Based on the permissions and features mentioned in the question and the game description, the sensitive permissions and features that should not be requested are:
-1. android.permission.WRITE_SETTINGS
-2. android.permission.CHANGE_CONFIGURATION
-3. android.permission.INJECT_EVENTS
-4. android.permission.REORDER_TASKS
-5. android.permission.BLUETOOTH
-6. android.permission.BLUETOOTH_ADMIN
-7. android.permission.WAKE_LOCK
-8. android.hardware.touchscreen (not required)
-9. android.hardware.touchscreen.multitouch (not required)
-10. android.hardware.touchscreen.multitouch.distinct (not required)
-11. android.hardware.vulkan.version (not required)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Based on the permissions and features mentioned, the following sensitive permissions and features should not be requested:
-Sensitive Permissions:
-- android.permission.INJECT_EVENTS (This permission allows injecting touch events and can potentially be used for malicious purposes)
-- android.permission.RECORD_AUDIO (This permission allows recording audio and can potentially infringe on privacy)
-- android.permission.WRITE_SETTINGS (This permission allows modifying system settings and can potentially be used for unauthorized modifications)
-Sensitive Features:
-- android.hardware.microphone (This feature indicates the availability of a microphone, which can potentially be used for recording audio without user consent)
-It is important to consider the privacy and security implications when requesting sensitive permissions and features in an app.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Based on the permissions and features mentioned, the sensitive permissions and features that should not be requested are:
-Sensitive Permissions:
-- android.permission.WRITE_SETTINGS
-- android.permission.CHANGE_CONFIGURATION
-- android.permission.INJECT_EVENTS
-- android.permission.REORDER_TASKS
-- android.permission.RECORD_AUDIO
-Sensitive Features:
-- android.hardware.microphone
-These permissions and features may not be necessary for the normal functioning of the game and could potentially compromise user privacy and security if granted.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Based on the information provided, the sensitive permissions that should not be requested are:
-- android.permission.WRITE_SETTINGS: This permission allows the app to modify system settings which can potentially be exploited for malicious purposes.
-- android.permission.REORDER_TASKS: This permission allows the app to reorder the tasks running in the system. It is not necessary for the functionality of a game and can potentially interfere with the user's multitasking experience.
-- android.permission.RECORD_AUDIO: This permission allows the app to record audio using the device's microphone. It is not necessary for the described gameplay and can be considered an invasion of privacy.
-- android.permission.BLUETOOTH: This permission allows the app to access Bluetooth functionality on the device. It is not mentioned in the game description and can be seen as unnecessary for a turn-based strategy and role-playing game.
-- android.permission.WRITE_EXTERNAL_STORAGE: This permission grants the app write access to the device's external storage. Since the game description does not mention any specific need for storage access, it is better not to request this permission to protect user data.
-- android.permission.READ_EXTERNAL_STORAGE: This permission grants the app read access to the device's external storage. Again, if not necessary for the game's functionality, it is recommended not to request this permission to protect user data.
-Regarding the features:
-- android.hardware.touchscreen: This feature is necessary for a game that involves interacting with the touchscreen.
-- android.hardware.touchscreen.multitouch: This feature is necessary for a game that supports multitouch input on the touchscreen.
-- android.hardware.touchscreen.multitouch.distinct: This feature indicates that the game supports distinct multitouch gestures, which can enhance gameplay experience.
-- android.hardware.microphone: This feature indicates that the game utilizes the device's microphone, likely for voice chat or voice input features.
-No specific features mentioned in the game description should not be requested.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>《Faraland》是一款回合 制策略和角色扮演游戏。在游戏中，你可以使用你的英雄，通过学习强大的技能、收集稀有装备、招募军队、在地图上运动、捕获资源和加入战斗来与其他玩家竞争。游戏的灵感来自魔兽世界、最终幻想故事情节、地平线零黎明背景、口袋妖怪和最终幻想战术战斗系统以及EVE在线游戏-玩家可以互相做任何事情。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="23" ns0:compileSdkVersionCodename="6.0-2438415" ns0:installLocation="auto" package="com.odders.ohshape.pico.neo2" platformBuildVersionCode="30" platformBuildVersionName="11"&gt;
+    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="29" ns0:compileSdkVersionCodename="10" ns0:installLocation="preferExternal" package="com.hunandamao.xiaochidian" platformBuildVersionCode="29" platformBuildVersionName="10"&gt;
     &lt;supports-screens ns0:anyDensity="true" ns0:largeScreens="true" ns0:normalScreens="true" ns0:smallScreens="true" ns0:xlargeScreens="true" /&gt;
+    &lt;uses-permission ns0:name="android.permission.ACCESS_NETWORK_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.INTERNET" /&gt;
+    &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_MULTICAST_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_EXTERNAL_STORAGE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_SETTINGS" /&gt;
+    &lt;uses-permission ns0:name="android.permission.READ_EXTERNAL_STORAGE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.REORDER_TASKS" /&gt;
+    &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.ACCESS_WIFI_STATE" /&gt;
     &lt;uses-feature ns0:glEsVersion="0x00030000" /&gt;
     &lt;uses-feature ns0:name="android.hardware.touchscreen" ns0:required="false" /&gt;
     &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch" ns0:required="false" /&gt;
     &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch.distinct" ns0:required="false" /&gt;
-    &lt;uses-permission ns0:name="android.permission.WRITE_SETTINGS" /&gt;
-    &lt;uses-permission ns0:name="android.permission.REORDER_TASKS" /&gt;
-    &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.INTERNET" /&gt;
-    &lt;uses-permission ns0:name="android.permission.ACCESS_NETWORK_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.ACCESS_WIFI_STATE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.RECORD_AUDIO" /&gt;
-    &lt;uses-permission ns0:name="android.permission.MODIFY_AUDIO_SETTINGS" /&gt;
-    &lt;uses-permission ns0:name="android.permission.BLUETOOTH" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.microphone" ns0:required="false" /&gt;
-    &lt;uses-permission ns0:name="android.permission.WRITE_EXTERNAL_STORAGE" /&gt;
-    &lt;uses-permission ns0:name="android.permission.READ_EXTERNAL_STORAGE" /&gt;
     &lt;application ns0:allowBackup="true" ns0:icon="@mipmap/app_icon" ns0:label="@string/app_name" ns0:requestLegacyExternalStorage="true" ns0:supportsRtl="true" ns0:usesCleartextTraffic="true"&gt;
+        &lt;meta-data ns0:name="unity.builder" ns0:value="\ 12369761376126" /&gt;
         &lt;activity ns0:configChanges="density|fontScale|keyboard|keyboardHidden|layoutDirection|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:launchMode="singleTask" ns0:name="com.unity3d.player.UnityPlayerActivity" ns0:screenOrientation="landscape" ns0:theme="@style/UnityThemeSelector"&gt;
             &lt;intent-filter&gt;
                 &lt;action ns0:name="android.intent.action.MAIN" /&gt;
@@ -2991,27 +2781,73 @@
         &lt;meta-data ns0:name="unity.splash-mode" ns0:value="0" /&gt;
         &lt;meta-data ns0:name="unity.splash-enable" ns0:value="true" /&gt;
         &lt;meta-data ns0:name="notch.config" ns0:value="portrait|landscape" /&gt;
-        &lt;meta-data ns0:name="unity.build-id" ns0:value="0ea0d07a-9d72-4946-8645-e39c1750c105" /&gt;
+        &lt;meta-data ns0:name="unity.build-id" ns0:value="c3dbb196-3f63-41ea-8111-f0eb3e5af3e5" /&gt;
         &lt;meta-data ns0:name="pvr.app.type" ns0:value="vr" /&gt;
-        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="XR Platform_2.0.4.3" /&gt;
+        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="XR Platform_1.2.4.7" /&gt;
         &lt;meta-data ns0:name="enable_cpt" ns0:value="0" /&gt;
-        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="1" /&gt;
-        &lt;meta-data ns0:name="pico_app_id" ns0:value="83a7cd05349ad5c38f5c8fa53466239b" /&gt;
-        &lt;meta-data ns0:name="pico_app_key" ns0:value="317b35cecd1fc75c3cb3e022deacd002" /&gt;
+        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="pico_merchant_id" ns0:value="5246" /&gt;
+        &lt;meta-data ns0:name="pico_app_id" ns0:value="c2a8870494a2005b73e87982f1f640aa" /&gt;
+        &lt;meta-data ns0:name="pico_app_key" ns0:value="16562ffe3bcedccd3da2395e50a8dc98" /&gt;
+        &lt;meta-data ns0:name="pico_pay_key" ns0:value="732f28f75f39fefd0a4262e640be0351" /&gt;
+        &lt;meta-data ns0:name="pico_app_id_foreign" ns0:value="81e6b29509fad6ee4cb9edb6b4e49d22" /&gt;
+        &lt;meta-data ns0:name="pico_app_key_foreign" ns0:value="03fa8d947440587acdb45e10939e5e31" /&gt;
+        &lt;meta-data ns0:name="pico_scope_foreign" ns0:value="get_user_info" /&gt;
+        &lt;meta-data ns0:name="pico_pay_key_foreign" ns0:value="bfbaeffa08e4bac4410482aa29d4e00b" /&gt;
+        &lt;meta-data ns0:name="pico_merchant_id_foreign" ns0:value="3653" /&gt;
+        &lt;meta-data ns0:name="pico_redirectUrl" ns0:value="http://www.picovr.com" /&gt;
         &lt;meta-data ns0:name="pico_scope" ns0:value="get_user_info" /&gt;
-        &lt;meta-data ns0:name="pico_pay_key" ns0:value="ae7b982818ff89a2f7b0fed2ffb4c048" /&gt;
-        &lt;meta-data ns0:name="pico_app_id_foreign" ns0:value="83a7cd05349ad5c38f5c8fa53466239b" /&gt;
-        &lt;meta-data ns0:name="pico_app_key_foreign" ns0:value="317b35cecd1fc75c3cb3e022deacd002" /&gt;
-        &lt;meta-data ns0:name="pico_scope_foreign" ns0:value="get_user_info" /&gt;
-        &lt;meta-data ns0:name="pico_pay_key_foreign" ns0:value="ae7b982818ff89a2f7b0fed2ffb4c048" /&gt;
+        &lt;meta-data ns0:name="com.pvr.instructionset" ns0:value="32" /&gt;
         &lt;activity ns0:excludeFromRecents="true" ns0:exported="true" ns0:launchMode="singleTask" ns0:name="com.pico.loginpaysdk.auth.TransferStationActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar"&gt;
             &lt;intent-filter&gt;
                 &lt;action ns0:name="com.pico.loginpaysdk.intent.action.AuthCallback" /&gt;
                 &lt;category ns0:name="android.intent.category.DEFAULT" /&gt;
             &lt;/intent-filter&gt;
         &lt;/activity&gt;
-        &lt;activity ns0:name="com.yasirkula.unity.NativeShareCustomShareDialogActivity" ns0:theme="@style/Theme.NativeShareTransparent" /&gt;
-        &lt;provider ns0:authorities="com.odders.ohshape.pico.neo2.NativeShareContentProvider" ns0:exported="false" ns0:grantUriPermissions="true" ns0:name="com.yasirkula.unity.NativeShareContentProvider" /&gt;
+    &lt;/application&gt;
+&lt;/manifest&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="29" ns0:compileSdkVersionCodename="10" ns0:installLocation="preferExternal" package="com.CharmingGame.EnterVR" platformBuildVersionCode="29" platformBuildVersionName="10"&gt;
+    &lt;supports-screens ns0:anyDensity="true" ns0:largeScreens="true" ns0:normalScreens="true" ns0:smallScreens="true" ns0:xlargeScreens="true" /&gt;
+    &lt;uses-feature ns0:glEsVersion="0x00020000" /&gt;
+    &lt;uses-permission ns0:name="android.permission.INTERNET" /&gt;
+    &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_MULTICAST_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_EXTERNAL_STORAGE" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.sensor.accelerometer" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.touchscreen" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch.distinct" ns0:required="false" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_SETTINGS" /&gt;
+    &lt;uses-permission ns0:name="android.permission.READ_EXTERNAL_STORAGE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.REORDER_TASKS" /&gt;
+    &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.ACCESS_NETWORK_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.ACCESS_WIFI_STATE" /&gt;
+    &lt;application ns0:allowBackup="true" ns0:icon="@mipmap/app_icon" ns0:label="@string/app_name" ns0:requestLegacyExternalStorage="true" ns0:supportsRtl="true"&gt;
+        &lt;activity ns0:configChanges="density|fontScale|keyboard|keyboardHidden|layoutDirection|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:launchMode="singleTask" ns0:name="com.unity3d.player.UnityPlayerActivity" ns0:screenOrientation="landscape" ns0:theme="@style/UnityThemeSelector"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="android.intent.action.MAIN" /&gt;
+                &lt;category ns0:name="android.intent.category.LAUNCHER" /&gt;
+            &lt;/intent-filter&gt;
+            &lt;meta-data ns0:name="unityplayer.UnityActivity" ns0:value="true" /&gt;
+            &lt;meta-data ns0:name="android.notch_support" ns0:value="true" /&gt;
+        &lt;/activity&gt;
+        &lt;meta-data ns0:name="unity.splash-mode" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="unity.splash-enable" ns0:value="true" /&gt;
+        &lt;meta-data ns0:name="notch.config" ns0:value="portrait|landscape" /&gt;
+        &lt;meta-data ns0:name="unity.build-id" ns0:value="6a9274e7-cc42-4866-8ca4-70caf29c4af9" /&gt;
+        &lt;meta-data ns0:name="pvr.app.type" ns0:value="vr" /&gt;
+        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="XR Platform_1.2.3.5" /&gt;
+        &lt;meta-data ns0:name="enable_cpt" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="0" /&gt;
+        &lt;activity ns0:excludeFromRecents="true" ns0:exported="true" ns0:launchMode="singleTask" ns0:name="com.pico.loginpaysdk.auth.TransferStationActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="com.pico.loginpaysdk.intent.action.AuthCallback" /&gt;
+                &lt;category ns0:name="android.intent.category.DEFAULT" /&gt;
+            &lt;/intent-filter&gt;
+        &lt;/activity&gt;
         &lt;activity ns0:configChanges="fontScale|keyboard|keyboardHidden|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="true" ns0:name="com.unity3d.services.ads.adunit.AdUnitActivity" ns0:theme="@android:style/Theme.NoTitleBar.Fullscreen" /&gt;
         &lt;activity ns0:configChanges="fontScale|keyboard|keyboardHidden|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="true" ns0:name="com.unity3d.services.ads.adunit.AdUnitTransparentActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar.Fullscreen" /&gt;
         &lt;activity ns0:configChanges="fontScale|keyboard|keyboardHidden|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:name="com.unity3d.services.ads.adunit.AdUnitTransparentSoftwareActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar.Fullscreen" /&gt;
@@ -3021,73 +2857,236 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Based on the permissions and features mentioned, the sensitive permissions and features that should not be requested are:
+    <t>Based on the permissions mentioned in the question, the sensitive permissions that should not be requested are:
+- android.permission.WRITE_SETTINGS: This permission allows the app to modify global system settings, which can be potentially harmful and intrusive to the user.
+Based on the features mentioned in the question, there are no sensitive features that should not be requested.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="29" ns0:compileSdkVersionCodename="10" ns0:installLocation="auto" package="com.scale1.sepsdinerSolo" platformBuildVersionCode="29" platformBuildVersionName="10"&gt;
+    &lt;supports-screens ns0:anyDensity="true" ns0:largeScreens="true" ns0:normalScreens="true" ns0:smallScreens="true" ns0:xlargeScreens="true" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_EXTERNAL_STORAGE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.READ_EXTERNAL_STORAGE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.BLUETOOTH" /&gt;
+    &lt;uses-permission ns0:name="android.permission.BLUETOOTH_ADMIN" /&gt;
+    &lt;uses-permission ns0:name="android.permission.INJECT_EVENTS" /&gt;
+    &lt;uses-permission ns0:name="android.permission.INTERNET" /&gt;
+    &lt;uses-permission ns0:name="android.permission.ACCESS_NETWORK_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.VIBRATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_SETTINGS" /&gt;
+    &lt;uses-permission ns0:name="android.permission.CHANGE_CONFIGURATION" /&gt;
+    &lt;uses-feature ns0:glEsVersion="0x00030000" /&gt;
+    &lt;uses-permission ns0:name="android.permission.RECORD_AUDIO" /&gt;
+    &lt;uses-permission ns0:name="android.permission.MODIFY_AUDIO_SETTINGS" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.microphone" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.sensor.accelerometer" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.touchscreen" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch.distinct" ns0:required="false" /&gt;
+    &lt;uses-permission ns0:name="android.permission.REORDER_TASKS" /&gt;
+    &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.ACCESS_WIFI_STATE" /&gt;
+    &lt;application ns0:allowBackup="true" ns0:debuggable="false" ns0:icon="@mipmap/app_icon" ns0:label="@string/app_name" ns0:requestLegacyExternalStorage="true" ns0:roundIcon="@mipmap/app_icon_round" ns0:supportsRtl="true" ns0:theme="@android:style/Theme.Black.NoTitleBar.Fullscreen"&gt;
+        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="Unity_2.8.9.12" /&gt;
+        &lt;meta-data ns0:name="pvr.app.type" ns0:value="vr" /&gt;
+        &lt;meta-data ns0:name="pvr.display.orientation" ns0:value="180" /&gt;
+        &lt;activity ns0:configChanges="density|fontScale|keyboard|keyboardHidden|layoutDirection|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:label="@string/app_name" ns0:launchMode="singleTask" ns0:name="com.unity3d.player.UnityPlayerNativeActivityPico" ns0:screenOrientation="landscape"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="android.intent.action.MAIN" /&gt;
+                &lt;category ns0:name="android.intent.category.LAUNCHER" /&gt;
+            &lt;/intent-filter&gt;
+            &lt;meta-data ns0:name="unityplayer.UnityActivity" ns0:value="true" /&gt;
+            &lt;meta-data ns0:name="unityplayer.ForwardNativeEventsToDalvik" ns0:value="false" /&gt;
+            &lt;meta-data ns0:name="android.notch_support" ns0:value="true" /&gt;
+        &lt;/activity&gt;
+        &lt;activity ns0:configChanges="keyboard|keyboardHidden|orientation|screenSize" ns0:name="com.pico.loginpaysdk.UnityAuthInterface" ns0:screenOrientation="landscape" /&gt;
+        &lt;activity ns0:configChanges="keyboardHidden|orientation" ns0:exported="false" ns0:name="com.pico.loginpaysdk.component.PicoSDKBrowser" ns0:windowSoftInputMode="adjustResize" /&gt;
+        &lt;service ns0:name="com.picovr.hummingbirdsvc.AutoConnectService"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="com.picovr.hummingbirdsvc.AutoConnectService" /&gt;
+            &lt;/intent-filter&gt;
+        &lt;/service&gt;
+        &lt;service ns0:name="com.picovr.picovrlib.hummingbird.HummingBirdControllerService" ns0:process=":remote"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="com.picovr.picovrlib.humingbird.HumingBirdAIDLService" /&gt;
+            &lt;/intent-filter&gt;
+        &lt;/service&gt;
+        &lt;meta-data ns0:name="com.pvr.instructionset" ns0:value="32" /&gt;
+        &lt;meta-data ns0:name="unityplayer.SkipPermissionsDialog" ns0:value="false" /&gt;
+        &lt;meta-data ns0:name="platform_logo" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="LoadingContent" ns0:resource="@string/loading" /&gt;
+        &lt;meta-data ns0:name="loadingcolor" ns0:resource="@color/custom" /&gt;
+        &lt;meta-data ns0:name="loadingtextsize" ns0:value="16" /&gt;
+        &lt;meta-data ns0:name="loadingwidth" ns0:value="500" /&gt;
+        &lt;meta-data ns0:name="loadingheight" ns0:value="100" /&gt;
+        &lt;meta-data ns0:name="loadingmarquee" ns0:value="1" /&gt;
+        &lt;meta-data ns0:name="bottommargin" ns0:value="100" /&gt;
+        &lt;meta-data ns0:name="marqueecount" ns0:value="10" /&gt;
+        &lt;meta-data ns0:name="loadingalign" ns0:value="left" /&gt;
+        &lt;meta-data ns0:name="com.pvr.hmd.trackingmode" ns0:value="6dof" /&gt;
+        &lt;meta-data ns0:name="isPUI" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="enable_eyetracking" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="enable_cpt" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="platform_high" ns0:value="1" /&gt;
+        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="1" /&gt;
+        &lt;meta-data ns0:name="pico_redirectUrl" ns0:value="http://www.picovr.com" /&gt;
+        &lt;meta-data ns0:name="pico_app_id" ns0:value="11638f51026498097f5a8938c9ee782a" /&gt;
+        &lt;meta-data ns0:name="pico_app_key" ns0:value="a9a79a522fa6fdb20a3a284ac3250769" /&gt;
+        &lt;meta-data ns0:name="pico_scope" ns0:value="get_user_info" /&gt;
+        &lt;meta-data ns0:name="pico_merchant_id" ns0:value="7230" /&gt;
+        &lt;meta-data ns0:name="pico_pay_key" ns0:value="af7153a5cdba32f20040b9b257f173a5" /&gt;
+        &lt;meta-data ns0:name="pico_app_id_foreign" ns0:value="11638f51026498097f5a8938c9ee782a" /&gt;
+        &lt;meta-data ns0:name="pico_app_key_foreign" ns0:value="a9a79a522fa6fdb20a3a284ac3250769" /&gt;
+        &lt;meta-data ns0:name="pico_scope_foreign" ns0:value="get_user_info" /&gt;
+        &lt;meta-data ns0:name="pico_merchant_id_foreign" ns0:value="7230" /&gt;
+        &lt;meta-data ns0:name="pico_pay_key_foreign" ns0:value="APP SECRET" /&gt;
+        &lt;meta-data ns0:name="unity.splash-mode" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="unity.splash-enable" ns0:value="true" /&gt;
+        &lt;meta-data ns0:name="notch.config" ns0:value="portrait|landscape" /&gt;
+        &lt;meta-data ns0:name="unity.build-id" ns0:value="ee1ef296-528d-4e67-834d-a02c999e78a8" /&gt;
+        &lt;activity ns0:excludeFromRecents="true" ns0:exported="true" ns0:launchMode="singleTask" ns0:name="com.pico.loginpaysdk.auth.TransferStationActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="com.pico.loginpaysdk.intent.action.AuthCallback" /&gt;
+                &lt;category ns0:name="android.intent.category.DEFAULT" /&gt;
+            &lt;/intent-filter&gt;
+        &lt;/activity&gt;
+    &lt;/application&gt;
+&lt;/manifest&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Based on the permissions and features mentioned, the following sensitive permissions and features should not be requested:
 Sensitive Permissions:
-1. android.permission.INJECT_EVENTS
-2. android.permission.RECORD_AUDIO
-3. android.permission.MODIFY_AUDIO_SETTINGS
-4. com.oculus.permission.HAND_TRACKING
+- android.permission.INJECT_EVENTS: This permission allows the app to inject user events, which can potentially be used for malicious purposes. It is not necessary for the functionality of a burger restaurant game.
 Sensitive Features:
-1. android.hardware.microphone (required="false")
-2. android.hardware.touchscreen (required="false")
-3. android.hardware.touchscreen.multitouch (required="false")
-4. android.hardware.touchscreen.multitouch.distinct (required="false")
-5. android.software.vr.mode (required="false")</t>
+None of the mentioned features are sensitive.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Based on the permissions and features mentioned in the question, the sensitive permissions and features that should not be requested for this game are:
-Sensitive Permissions:
-1. android.permission.RECORD_AUDIO - This permission is not necessary for the gameplay described in the game description.
-Sensitive Features:
-1. android.hardware.microphone - This feature is not necessary for the gameplay described in the game description.</t>
+    <t>欢迎来到 Sep’s Diner，这是一家由您担任主厨的新汉堡餐厅！它真的会成为镇上最好的汉堡吗？现在就看你了！一层又一层，您的体验将增加，美食客户的数量也会增加。他们很匆忙，所以在他们离开之前尽快满足他们！
+饥饿和不耐烦，他们不会让您犯错误…… 细心和精确，以获得最大的利润！包括全新的甜点餐厅Sep’s Donut！游戏特色：· 2间餐厅· 包括 3 种游戏模式：定时、轻松、多人· 每家餐厅包括 27 个级别（定时/休闲 12 个，多人游戏 3 个）· 最多 4 名玩家的多人合作游戏· 紧张刺激的关卡！· 身临其境的音频氛围· 不耐烦的客户用有趣的声音· 美丽的风景和彩灯· 逐级增加难度· 超过 30 种不同的汉堡食谱组合！· 煎饼、甜甜圈、华夫饼、纸杯蛋糕、冰淇淋和奶昔！</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OhShape是一款能够带来独一无二全身活动的音乐节奏类游戏。每张地图都需要躲避障碍，打击墙壁和做出可爱造型。通过游戏获取奖励，做自己的超级明星。 官方支持定制歌曲 享受前所未有的畅快感觉，享受无穷无尽的快乐。 OhShape给所有家庭带来快乐。通过4个不同难度的关卡和许多游戏设置，您能够定制适合自己技术的体验，并且感受不断练习带来的提升。
-游戏关键词：体育、音乐
-游戏特色：
-• 充满乐趣的全身锻炼体验
-• 32个精雕细琢关卡，4个不同难度
-• 派对模式：和家人，朋友一起参与游戏
-• 练习模式：联系关卡中的一个片段
-• 为最活跃用户提供的挑战模式
-• 容易上手的定制歌曲关卡编辑器
-• 跨平台在线排行榜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Open Brush 汉化中文版，支持Quest一体机、Pico3、Pico4一体机设备  
-《Tilt Brush》倾斜的刷子(画画神器) 升级版，和谷歌VR绘画一样，功能还多了些，比如可以开启透视功能实现MR混合现实绘画。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Based on the given information, the sensitive permissions and features that should not be requested for this game are:
+    <t>Based on the given information, the following sensitive permissions and features should not be requested:
 Permissions:
-- android.permission.CAMERA
+- android.permission.BLUETOOTH
+- android.permission.BLUETOOTH_ADMIN
 - android.permission.RECORD_AUDIO
 - android.permission.MODIFY_AUDIO_SETTINGS
-- android.permission.BLUETOOTH
+- android.permission.READ_EXTERNAL_STORAGE
 - android.permission.WRITE_EXTERNAL_STORAGE
+- android.permission.INJECT_EVENTS
 - android.permission.WRITE_SETTINGS
-- vive.wave.vr.oem.data.OEMDataRead
-- vive.wave.vr.oem.data.OEMDataWrite
-- android.permission.BLUETOOTH_CONNECT
+- android.permission.CHANGE_WIFI_STATE
+- android.permission.CHANGE_CONFIGURATION
+- android.permission.REORDER_TASKS
 Features:
-- android.hardware.camera
-- android.hardware.camera.autofocus
-- android.hardware.camera.front
-- android.hardware.microphone</t>
+- android.hardware.microphone
+- android.hardware.touchscreen
+- android.hardware.touchscreen.multitouch
+- android.hardware.touchscreen.multitouch.distinct</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;uses-permission ns0:name="android.permission.CAMERA" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.camera" ns0:required="false" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.camera.autofocus" ns0:required="false" /&gt;
-    &lt;uses-feature ns0:name="android.hardware.camera.front" ns0:required="false" /&gt;
-    &lt;uses-permission ns0:name="android.permission.RECORD_AUDIO" /&gt;
-    &lt;uses-permission ns0:name="android.permission.MODIFY_AUDIO_SETTINGS" /&gt;
- &lt;uses-feature ns0:name="android.hardware.microphone" ns0:required="false" /&gt;</t>
+    <t>云端高尔夫建立在玩和迷你高尔夫球场的乐趣之上，带有1000多个部件的关卡编辑器，用于构建和制作史诗般的迷你高尔夫球场或完整的高尔夫球洞。
+并增加了玩全尺寸高尔夫球场的能力。用推杆，挖起杆和驱动器武装自己，并击中云端的链接。-54洞单人战役将带您穿越绿色林地，魔幻草地和收割者废墟。打18号洞的全尺寸高尔夫球和迷你高尔夫球。-带有1000多个部件的关卡编辑器，用于构建和制作史诗般的迷你高尔夫球场或完整的高尔夫球洞。创建并上传您的作品，以允许其他人玩。-期望找到惊人的用户创建的关卡几乎无限的供应。现有的所有Cloudlands 1孔都可以使用（2000多个）。-在线多人游戏最多允许4位玩家一起玩。创建一个房间，让您的朋友加入，然后离开。-本地多人游戏的传递和播放功能允许您和您的朋友通过在您之间传递一个耳机来一起玩。-完全支持游戏内语音聊天和Oculus Avatars。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Based on the provided information, the sensitive permissions and features that should NOT be requested are:
+- android.permission.INJECT_EVENTS
+- android.permission.REORDER_TASKS
+- android.permission.RECORD_AUDIO
+- android.hardware.microphone (required: false)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;manifest xmlns:ns0="http://schemas.android.com/apk/res/android" ns0:compileSdkVersion="29" ns0:compileSdkVersionCodename="10" ns0:installLocation="auto" package="com.IvanovichGames.BeatBlaster" platformBuildVersionCode="29" platformBuildVersionName="10"&gt;
+    &lt;supports-screens ns0:anyDensity="true" ns0:largeScreens="true" ns0:normalScreens="true" ns0:smallScreens="true" ns0:xlargeScreens="true" /&gt;
+    &lt;uses-permission ns0:name="android.permission.INTERNET" /&gt;
+    &lt;uses-permission ns0:name="android.permission.ACCESS_NETWORK_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.VIBRATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_EXTERNAL_STORAGE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.READ_EXTERNAL_STORAGE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WRITE_SETTINGS" /&gt;
+    &lt;uses-permission ns0:name="android.permission.CHANGE_CONFIGURATION" /&gt;
+    &lt;uses-permission ns0:name="android.permission.BLUETOOTH" /&gt;
+    &lt;uses-permission ns0:name="android.permission.BLUETOOTH_ADMIN" /&gt;
+    &lt;uses-permission ns0:name="android.permission.INJECT_EVENTS" /&gt;
+    &lt;uses-feature ns0:glEsVersion="0x00030000" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.vulkan.version" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.touchscreen" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch" ns0:required="false" /&gt;
+    &lt;uses-feature ns0:name="android.hardware.touchscreen.multitouch.distinct" ns0:required="false" /&gt;
+    &lt;uses-permission ns0:name="android.permission.REORDER_TASKS" /&gt;
+    &lt;uses-permission ns0:name="android.permission.CHANGE_WIFI_STATE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.ACCESS_WIFI_STATE" /&gt;
+    &lt;uses-permission ns0:name="com.android.vending.CHECK_LICENSE" /&gt;
+    &lt;uses-permission ns0:name="android.permission.WAKE_LOCK" /&gt;
+    &lt;application ns0:allowBackup="true" ns0:debuggable="false" ns0:extractNativeLibs="true" ns0:icon="@mipmap/app_icon" ns0:label="@string/app_name" ns0:requestLegacyExternalStorage="true" ns0:roundIcon="@mipmap/app_icon_round" ns0:supportsRtl="true" ns0:theme="@android:style/Theme.Black.NoTitleBar.Fullscreen"&gt;
+        &lt;meta-data ns0:name="pvr.sdk.version" ns0:value="Unity_2.8.9.12" /&gt;
+        &lt;meta-data ns0:name="pvr.app.type" ns0:value="vr" /&gt;
+        &lt;meta-data ns0:name="pvr.display.orientation" ns0:value="180" /&gt;
+        &lt;activity ns0:configChanges="density|fontScale|keyboard|keyboardHidden|layoutDirection|locale|mcc|mnc|navigation|orientation|screenLayout|screenSize|smallestScreenSize|touchscreen|uiMode" ns0:hardwareAccelerated="false" ns0:label="@string/app_name" ns0:launchMode="singleTask" ns0:name="com.unity3d.player.UnityPlayerNativeActivityPico" ns0:resizeableActivity="false" ns0:screenOrientation="landscape"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="android.intent.action.MAIN" /&gt;
+                &lt;category ns0:name="android.intent.category.LAUNCHER" /&gt;
+            &lt;/intent-filter&gt;
+            &lt;meta-data ns0:name="unityplayer.UnityActivity" ns0:value="true" /&gt;
+            &lt;meta-data ns0:name="unityplayer.ForwardNativeEventsToDalvik" ns0:value="false" /&gt;
+        &lt;/activity&gt;
+        &lt;activity ns0:configChanges="keyboard|keyboardHidden|orientation|screenSize" ns0:name="com.pico.loginpaysdk.UnityAuthInterface" ns0:screenOrientation="landscape" /&gt;
+        &lt;activity ns0:configChanges="keyboardHidden|orientation" ns0:exported="false" ns0:name="com.pico.loginpaysdk.component.PicoSDKBrowser" ns0:windowSoftInputMode="adjustResize" /&gt;
+        &lt;service ns0:name="com.picovr.hummingbirdsvc.AutoConnectService"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="com.picovr.hummingbirdsvc.AutoConnectService" /&gt;
+            &lt;/intent-filter&gt;
+        &lt;/service&gt;
+        &lt;service ns0:name="com.picovr.picovrlib.hummingbird.HummingBirdControllerService" ns0:process=":remote"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="com.picovr.picovrlib.humingbird.HumingBirdAIDLService" /&gt;
+            &lt;/intent-filter&gt;
+        &lt;/service&gt;
+        &lt;meta-data ns0:name="pico_merchant_id" ns0:value="81" /&gt;
+        &lt;meta-data ns0:name="pico_app_id" ns0:value="56898ecfc4a8f01dc518016fb7b1c0bc" /&gt;
+        &lt;meta-data ns0:name="pico_app_key" ns0:value="dc349716a16d8ef8061f8b62750c85ad" /&gt;
+        &lt;meta-data ns0:name="pico_pay_key" ns0:value="7f0c28552ea4427c03b67fdd66cf7e55" /&gt;
+        &lt;meta-data ns0:name="pico_redirectUrl" ns0:value="http://www.picovr.com" /&gt;
+        &lt;meta-data ns0:name="pico_scope" ns0:value="get_user_info" /&gt;
+        &lt;meta-data ns0:name="com.pvr.instructionset" ns0:value="32" /&gt;
+        &lt;meta-data ns0:name="platform_logo" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="LoadingContent" ns0:resource="@string/loading" /&gt;
+        &lt;meta-data ns0:name="loadingcolor" ns0:resource="@color/custom" /&gt;
+        &lt;meta-data ns0:name="loadingtextsize" ns0:value="16" /&gt;
+        &lt;meta-data ns0:name="loadingwidth" ns0:value="500" /&gt;
+        &lt;meta-data ns0:name="loadingheight" ns0:value="100" /&gt;
+        &lt;meta-data ns0:name="loadingmarquee" ns0:value="1" /&gt;
+        &lt;meta-data ns0:name="bottommargin" ns0:value="100" /&gt;
+        &lt;meta-data ns0:name="marqueecount" ns0:value="10" /&gt;
+        &lt;meta-data ns0:name="loadingalign" ns0:value="left" /&gt;
+        &lt;meta-data ns0:name="com.pvr.hmd.trackingmode" ns0:value="6dof" /&gt;
+        &lt;meta-data ns0:name="isPUI" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="enable_eyetracking" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="enable_cpt" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="platform_high" ns0:value="1" /&gt;
+        &lt;meta-data ns0:name="enable_entitlementcheck" ns0:value="1" /&gt;
+        &lt;meta-data ns0:name="MSAA" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="unity.splash-mode" ns0:value="0" /&gt;
+        &lt;meta-data ns0:name="unity.splash-enable" ns0:value="true" /&gt;
+        &lt;meta-data ns0:name="unity.allow-resizable-window" ns0:value="false" /&gt;
+        &lt;meta-data ns0:name="unity.build-id" ns0:value="b8492c8a-f3aa-4abf-a368-2c6ccb496c52" /&gt;
+        &lt;activity ns0:excludeFromRecents="true" ns0:exported="true" ns0:launchMode="singleTask" ns0:name="com.pico.loginpaysdk.auth.TransferStationActivity" ns0:theme="@android:style/Theme.Translucent.NoTitleBar"&gt;
+            &lt;intent-filter&gt;
+                &lt;action ns0:name="com.pico.loginpaysdk.intent.action.AuthCallback" /&gt;
+                &lt;category ns0:name="android.intent.category.DEFAULT" /&gt;
+            &lt;/intent-filter&gt;
+        &lt;/activity&gt;
+        &lt;activity ns0:name="com.unity3d.plugin.downloader.UnityDownloaderActivity" /&gt;
+        &lt;service ns0:name="com.unity3d.plugin.downloader.UnityDownloaderService" /&gt;
+        &lt;receiver ns0:name="com.unity3d.plugin.downloader.UnityAlarmReceiver" /&gt;
+    &lt;/application&gt;
+&lt;/manifest&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3181,65 +3180,42 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>【游戏名称】：Space Fitness
-【游戏类型】：运动
-【游戏平台】：pico
-【游戏模式】：原生VR游戏（定位控制器）
-【游戏语言】：多国语言
-【游戏容量】：143MB
-【游戏介绍】：
-关于这款游戏
-在太空中，飞船突发意外，你需要几岁各式各样的陨石来通过不同挑战。
-《太空健身计划》集健身与游戏于一体，在这个广阔的太空中，你可以享受无限挑战乐趣。</t>
+    <t>Based on the permissions and features mentioned in the question and the game description, the sensitive permissions and features that should not be requested are:
+Sensitive Permissions:
+- android.permission.INJECT_EVENTS
+- android.permission.REORDER_TASKS
+Sensitive Features:
+None mentioned in the question or game description.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>VR驾校是一款练车神器！
-是学车的好帮手，让我们更快的学会驾驶。
-动态色彩标线辅助练车
-什么是车感？就是在车内对外部环境的距离感知，有的人距离感强，很快就能练成，有的人距离感弱，需要更长的时间；大多数人对距离不敏感，但是对色彩却很敏感，根据这一特点我们设计了一整套动态色彩练车系统：红色表示当前车距离“标线的标准位置”差距很大；绿色表示当前车距离“标线的标准位置”相差无几，是下一步操作时机。 当前车的位置越标准越绿，越不标准越红。</t>
+    <t>在太空竞技场中生存，使用各种武器消灭所有敌人！
+准备好在我们的手机游戏中进行激动人心的太空冒险！您将降落在太空音乐舞台上，与来自不同方面的敌人作战。使用激光和导弹等炫酷武器击败它们并避开敌方火箭！
+加入独特的挑战。你能成为顶级太空战士吗？立即下载游戏并尝试一下！
+**游戏特色**
+- 许多武器 |使用各种不同类型的武器。手枪、激光、枪支和火箭！
+- 近战武器 |不喜欢射击？使用剑！
+- 太空音乐竞技场 |使用耳机，享受美妙的节拍和音乐！
+- 挑战 |游戏中有首领，您有足够的勇气与他们战斗吗？
+- 更新 |我们将每月更新我们的游戏，为您带来新的内容。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>单人游戏，而且需要使用摄像头来与外界互动。
-【名称】：Squingle VR
-【类型】：解密/益智
-【平台】：Oculus Quest &amp; 二代
-【联机】：单人离线
-【大小】：360MB
-【刷新】：90Hz
-【语言】：英文
-【说明】：
-在时间之前只有 Squingle – 她需要你的帮助来创造宇宙！
-引导旋转球体穿过 100 个手工制作的、扭曲和旋转的彩虹色迷宫，然后与自己的幽灵赛跑！
-通过不断变化的音乐音景和“属于自己的迷幻视觉效果”解决巧妙的难题。你会发现 Squinle 的意思吗？
-“将成为VR历史上的经典！”
-“充满风格，独特而令人敬畏”
-“玩起来超级满足”
-“客观上是 Quest 2 上一些最好的图形和声音”</t>
+    <t>在《Discovery》, 你可以探索一个能够自由创作的巨大世界。你将能够构建属于自己的房子，村庄，城市，纪念性地标甚至挖掘深不见底的地下世界。明亮的火把会在夜幕来临时照亮你自豪的作品，而你也会欣赏到美丽的日落和夜空的繁星。伴随着达60FPS的高品质画面以及逼真的光线和阴影，在巨大的沙盒世界里，一天内不同时间点的场景变化都是那么地充满沉浸感。欣赏澎湃的音乐，引爆那必不可少的炸药！ 更多的功能和玩法正在持续更新中。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Based on the provided information, the sensitive permissions and features that should not be requested for this game are:
-1. Permissions:
-- vive.wave.vr.oem.data.OEMDataRead
-- vive.wave.vr.oem.data.OEMDataWrite
-2. Features:
-- N/A (All the mentioned features are relevant for the game)</t>
+    <t>Based on the permissions and features mentioned in the question, the sensitive permissions and features that should not be requested are:
+- android.permission.INJECT_EVENTS
+- android.permission.CHANGE_WIFI_MULTICAST_STATE
+- android.permission.MODIFY</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>一场这是一个多人联机游戏。比赛10项运动！
-■ 丰富的运动项目体验
--棒球、射箭、乒乓球、篮球、保龄球、羽毛球、高尔夫、飞镖、台球、拳击
-■ 多人实时PvP
--拳击、棒球和乒乓球还不受支持
-■ 通过高级物理实现逼真的虚拟运动体验
-■ 播放器定制
-■ 简单的用户界面和简单的控制可以帮助任何人玩
-■ 从初学者到专业人士有5种不同的困难
-*比赛形式与奥运会官方规则相同，因此你可以学习运动训练和规则。
-*适用于由于体育设施和天气条件而必须在室内进行的虚拟现实体育教室。</t>
+    <t>Based on the permissions and features mentioned, the sensitive permissions and features that should not be requested are:
+- android.permission.INJECT_EVENTS
+- android.permission.RECORD_AUDIO
+- android.hardware.microphone</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3286,7 +3262,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3320,6 +3296,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3532,7 +3514,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6372,7 +6354,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6406,33 +6388,33 @@
         <v>108</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>402</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>379</v>
+        <v>109</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>382</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>397</v>
+        <v>110</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>383</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>384</v>
+      </c>
+      <c r="E3" s="31" t="s">
         <v>111</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>380</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6440,50 +6422,50 @@
         <v>114</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>398</v>
+        <v>115</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>381</v>
+        <v>116</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>119</v>
+        <v>386</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>122</v>
+        <v>387</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6491,135 +6473,135 @@
         <v>123</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>124</v>
+        <v>391</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>125</v>
+        <v>389</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>127</v>
+        <v>398</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>385</v>
+        <v>397</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>128</v>
+        <v>395</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>386</v>
+        <v>393</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>392</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>109</v>
+        <v>396</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>387</v>
+        <v>399</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>394</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>389</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>388</v>
+        <v>132</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>401</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>390</v>
+        <v>133</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D13" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="B13" s="31" t="s">
-        <v>393</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>392</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>136</v>
-      </c>
       <c r="E13" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="B14" s="31" t="s">
-        <v>394</v>
-      </c>
       <c r="C14" s="31" t="s">
-        <v>395</v>
+        <v>143</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>144</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6627,84 +6609,84 @@
         <v>145</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>400</v>
+        <v>146</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>401</v>
+        <v>147</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>396</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>399</v>
+        <v>151</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>153</v>
+        <v>368</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="C18" t="s">
-        <v>157</v>
+        <v>159</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>367</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>159</v>
+        <v>369</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="C19" t="s">
         <v>162</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>370</v>
       </c>
       <c r="D19" s="31" t="s">
         <v>163</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6714,105 +6696,103 @@
       <c r="B20" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="31" t="s">
+        <v>371</v>
+      </c>
+      <c r="D20" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="D20" s="31" t="s">
-        <v>167</v>
-      </c>
       <c r="E20" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="C21" s="31" t="s">
+        <v>372</v>
+      </c>
+      <c r="D21" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="C21" t="s">
-        <v>170</v>
-      </c>
-      <c r="D21" s="31" t="s">
-        <v>171</v>
-      </c>
       <c r="E21" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>373</v>
+      </c>
+      <c r="D22" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B22" s="31" t="s">
-        <v>173</v>
-      </c>
-      <c r="C22" t="s">
-        <v>174</v>
-      </c>
-      <c r="D22" s="31" t="s">
-        <v>175</v>
-      </c>
       <c r="E22" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>380</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="C24" t="s">
-        <v>181</v>
+        <v>381</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>376</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>183</v>
+        <v>378</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="C25" t="s">
-        <v>185</v>
+        <v>379</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>377</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E25" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E27" s="31" t="s">
-        <v>376</v>
-      </c>
+      <c r="E27" s="31"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -6840,7 +6820,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7014,7 +6994,7 @@
         <v>74</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7176,10 +7156,10 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7187,10 +7167,10 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7198,10 +7178,10 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7209,10 +7189,10 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7220,10 +7200,10 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7231,10 +7211,10 @@
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7242,10 +7222,10 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7253,10 +7233,10 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7264,10 +7244,10 @@
         <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7275,10 +7255,10 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7286,10 +7266,10 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7297,10 +7277,10 @@
         <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7308,10 +7288,10 @@
         <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7319,10 +7299,10 @@
         <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7330,10 +7310,10 @@
         <v>15</v>
       </c>
       <c r="B47" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7341,10 +7321,10 @@
         <v>16</v>
       </c>
       <c r="B48" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7352,10 +7332,10 @@
         <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7363,10 +7343,10 @@
         <v>18</v>
       </c>
       <c r="B50" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7374,10 +7354,10 @@
         <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7385,10 +7365,10 @@
         <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -7443,20 +7423,20 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -7466,7 +7446,7 @@
         <v>45</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D9" s="15"/>
     </row>
@@ -7475,16 +7455,16 @@
         <v>48</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D11" s="19"/>
     </row>
@@ -7492,83 +7472,83 @@
     <row r="13" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:1" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:1" s="9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:1" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:1" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="29" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:1" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="G35" s="23" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -10664,692 +10644,692 @@
   <sheetData>
     <row r="1" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>